<commit_message>
Data added, Thesis modified.
</commit_message>
<xml_diff>
--- a/MetricConvergence.xlsx
+++ b/MetricConvergence.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr showInkAnnotation="0" defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tghad\OneDrive\Documents\GitHub\TarekGhaddarMastersWork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tghaddar/TarekGhaddarMastersWork/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" tabRatio="500"/>
+    <workbookView xWindow="6080" yWindow="3820" windowWidth="24740" windowHeight="19500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Opposite Pins" sheetId="1" r:id="rId1"/>
-    <sheet name="Same Side Pins" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Same Side Pins" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="for_spreadsheet" localSheetId="1">Sheet2!$A$1:$K$19</definedName>
+  </definedNames>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,8 +28,30 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="for_spreadsheet" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Volumes/tghaddar/PDTCurrent/restapl-pdt/pdt/inputs/ConvergenceInputs/for_spreadsheet.csv" comma="1">
+      <textFields count="11">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="13">
   <si>
     <t>Area</t>
   </si>
@@ -62,11 +88,14 @@
   <si>
     <t>Coarse</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -122,7 +151,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -139,9 +168,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +192,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="for_spreadsheet" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -214,9 +244,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -249,9 +279,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -433,31 +463,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:U20"/>
+    <sheetView showRuler="0" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.125" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="13.625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2429,26 +2459,708 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1.8536600000000001</v>
+      </c>
+      <c r="C2">
+        <v>1.36134</v>
+      </c>
+      <c r="D2">
+        <v>1.76471</v>
+      </c>
+      <c r="E2">
+        <v>1.47929</v>
+      </c>
+      <c r="F2">
+        <v>1.74194</v>
+      </c>
+      <c r="G2">
+        <v>1.59535</v>
+      </c>
+      <c r="H2">
+        <v>1.792</v>
+      </c>
+      <c r="I2">
+        <v>1.8202199999999999</v>
+      </c>
+      <c r="J2">
+        <v>1.9230799999999999</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1.8</v>
+      </c>
+      <c r="B3">
+        <v>1.14513</v>
+      </c>
+      <c r="C3">
+        <v>1.32582</v>
+      </c>
+      <c r="D3">
+        <v>1.65079</v>
+      </c>
+      <c r="E3">
+        <v>2.0833300000000001</v>
+      </c>
+      <c r="F3">
+        <v>2.5814900000000001</v>
+      </c>
+      <c r="G3">
+        <v>2.4088699999999998</v>
+      </c>
+      <c r="H3">
+        <v>2.68729</v>
+      </c>
+      <c r="I3">
+        <v>3.8282099999999999</v>
+      </c>
+      <c r="J3">
+        <v>3.9929000000000001</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1.6</v>
+      </c>
+      <c r="B4">
+        <v>1.1231899999999999</v>
+      </c>
+      <c r="C4">
+        <v>1.34416</v>
+      </c>
+      <c r="D4">
+        <v>1.65079</v>
+      </c>
+      <c r="E4">
+        <v>2.3480699999999999</v>
+      </c>
+      <c r="F4">
+        <v>2.67008</v>
+      </c>
+      <c r="G4">
+        <v>2.47139</v>
+      </c>
+      <c r="H4">
+        <v>2.9592000000000001</v>
+      </c>
+      <c r="I4">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="J4">
+        <v>2.9729700000000001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1.4</v>
+      </c>
+      <c r="B5">
+        <v>1.1216200000000001</v>
+      </c>
+      <c r="C5">
+        <v>1.36758</v>
+      </c>
+      <c r="D5">
+        <v>1.7885200000000001</v>
+      </c>
+      <c r="E5">
+        <v>1.8594999999999999</v>
+      </c>
+      <c r="F5">
+        <v>1.82741</v>
+      </c>
+      <c r="G5">
+        <v>2.7080299999999999</v>
+      </c>
+      <c r="H5">
+        <v>2.8167900000000001</v>
+      </c>
+      <c r="I5">
+        <v>2.57803</v>
+      </c>
+      <c r="J5">
+        <v>3.74288</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1.2</v>
+      </c>
+      <c r="B6">
+        <v>1.1527400000000001</v>
+      </c>
+      <c r="C6">
+        <v>1.5044</v>
+      </c>
+      <c r="D6">
+        <v>1.53975</v>
+      </c>
+      <c r="E6">
+        <v>1.5625</v>
+      </c>
+      <c r="F6">
+        <v>1.7059500000000001</v>
+      </c>
+      <c r="G6">
+        <v>2.13496</v>
+      </c>
+      <c r="H6">
+        <v>2.8054800000000002</v>
+      </c>
+      <c r="I6">
+        <v>2.7930999999999999</v>
+      </c>
+      <c r="J6">
+        <v>2.8664999999999998</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1.1451199999999999</v>
+      </c>
+      <c r="C7">
+        <v>1.4464300000000001</v>
+      </c>
+      <c r="D7">
+        <v>1.73285</v>
+      </c>
+      <c r="E7">
+        <v>1.7373400000000001</v>
+      </c>
+      <c r="F7">
+        <v>1.73767</v>
+      </c>
+      <c r="G7">
+        <v>2.3857699999999999</v>
+      </c>
+      <c r="H7">
+        <v>2.4763500000000001</v>
+      </c>
+      <c r="I7">
+        <v>2.8114400000000002</v>
+      </c>
+      <c r="J7">
+        <v>3.0713599999999999</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.8</v>
+      </c>
+      <c r="B8">
+        <v>1.13913</v>
+      </c>
+      <c r="C8">
+        <v>1.4017200000000001</v>
+      </c>
+      <c r="D8">
+        <v>1.4662599999999999</v>
+      </c>
+      <c r="E8">
+        <v>1.4446600000000001</v>
+      </c>
+      <c r="F8">
+        <v>1.5845100000000001</v>
+      </c>
+      <c r="G8">
+        <v>2.2559900000000002</v>
+      </c>
+      <c r="H8">
+        <v>2.3832900000000001</v>
+      </c>
+      <c r="I8">
+        <v>2.5979999999999999</v>
+      </c>
+      <c r="J8">
+        <v>3.3932099999999998</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0.6</v>
+      </c>
+      <c r="B9">
+        <v>1.0531600000000001</v>
+      </c>
+      <c r="C9">
+        <v>1.3052299999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.49264</v>
+      </c>
+      <c r="E9">
+        <v>1.8511</v>
+      </c>
+      <c r="F9">
+        <v>1.5726800000000001</v>
+      </c>
+      <c r="G9">
+        <v>1.81481</v>
+      </c>
+      <c r="H9">
+        <v>1.8073900000000001</v>
+      </c>
+      <c r="I9">
+        <v>2.4187500000000002</v>
+      </c>
+      <c r="J9">
+        <v>2.3648600000000002</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.4</v>
+      </c>
+      <c r="B10">
+        <v>1.09456</v>
+      </c>
+      <c r="C10">
+        <v>1.1939900000000001</v>
+      </c>
+      <c r="D10">
+        <v>1.36528</v>
+      </c>
+      <c r="E10">
+        <v>1.7741</v>
+      </c>
+      <c r="F10">
+        <v>1.7123699999999999</v>
+      </c>
+      <c r="G10">
+        <v>1.8666700000000001</v>
+      </c>
+      <c r="H10">
+        <v>1.5737699999999999</v>
+      </c>
+      <c r="I10">
+        <v>1.7179199999999999</v>
+      </c>
+      <c r="J10">
+        <v>2.2575699999999999</v>
+      </c>
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.2</v>
+      </c>
+      <c r="B11">
+        <v>1.0562100000000001</v>
+      </c>
+      <c r="C11">
+        <v>1.1480999999999999</v>
+      </c>
+      <c r="D11">
+        <v>1.18482</v>
+      </c>
+      <c r="E11">
+        <v>1.3494999999999999</v>
+      </c>
+      <c r="F11">
+        <v>1.62737</v>
+      </c>
+      <c r="G11">
+        <v>1.67045</v>
+      </c>
+      <c r="H11">
+        <v>1.73326</v>
+      </c>
+      <c r="I11">
+        <v>1.5178499999999999</v>
+      </c>
+      <c r="J11">
+        <v>1.71723</v>
+      </c>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.1</v>
+      </c>
+      <c r="B12">
+        <v>1.02349</v>
+      </c>
+      <c r="C12">
+        <v>1.0375399999999999</v>
+      </c>
+      <c r="D12">
+        <v>1.1470199999999999</v>
+      </c>
+      <c r="E12">
+        <v>1.2188300000000001</v>
+      </c>
+      <c r="F12">
+        <v>1.2861199999999999</v>
+      </c>
+      <c r="G12">
+        <v>1.33558</v>
+      </c>
+      <c r="H12">
+        <v>1.2548999999999999</v>
+      </c>
+      <c r="I12">
+        <v>1.25709</v>
+      </c>
+      <c r="J12">
+        <v>1.3713900000000001</v>
+      </c>
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>0.08</v>
+      </c>
+      <c r="B13">
+        <v>1.0143200000000001</v>
+      </c>
+      <c r="C13">
+        <v>1.0368200000000001</v>
+      </c>
+      <c r="D13">
+        <v>1.0849800000000001</v>
+      </c>
+      <c r="E13">
+        <v>1.1451100000000001</v>
+      </c>
+      <c r="F13">
+        <v>1.20323</v>
+      </c>
+      <c r="G13">
+        <v>1.29548</v>
+      </c>
+      <c r="H13">
+        <v>1.2228300000000001</v>
+      </c>
+      <c r="I13">
+        <v>1.20896</v>
+      </c>
+      <c r="J13">
+        <v>1.25722</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>0.06</v>
+      </c>
+      <c r="B14">
+        <v>1.00759</v>
+      </c>
+      <c r="C14">
+        <v>1.03349</v>
+      </c>
+      <c r="D14">
+        <v>1.0370699999999999</v>
+      </c>
+      <c r="E14">
+        <v>1.10328</v>
+      </c>
+      <c r="F14">
+        <v>1.0844400000000001</v>
+      </c>
+      <c r="G14">
+        <v>1.2034800000000001</v>
+      </c>
+      <c r="H14">
+        <v>1.17547</v>
+      </c>
+      <c r="I14">
+        <v>1.26431</v>
+      </c>
+      <c r="J14">
+        <v>1.1868300000000001</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>0.05</v>
+      </c>
+      <c r="B15">
+        <v>1.0159199999999999</v>
+      </c>
+      <c r="C15">
+        <v>1.02633</v>
+      </c>
+      <c r="D15">
+        <v>1.0484500000000001</v>
+      </c>
+      <c r="E15">
+        <v>1.0731200000000001</v>
+      </c>
+      <c r="F15">
+        <v>1.0606899999999999</v>
+      </c>
+      <c r="G15">
+        <v>1.12141</v>
+      </c>
+      <c r="H15">
+        <v>1.14801</v>
+      </c>
+      <c r="I15">
+        <v>1.2327399999999999</v>
+      </c>
+      <c r="J15">
+        <v>1.15544</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>0.04</v>
+      </c>
+      <c r="B16">
+        <v>1.0027699999999999</v>
+      </c>
+      <c r="C16">
+        <v>1.02755</v>
+      </c>
+      <c r="D16">
+        <v>1.00502</v>
+      </c>
+      <c r="E16">
+        <v>1.05935</v>
+      </c>
+      <c r="F16">
+        <v>1.0763400000000001</v>
+      </c>
+      <c r="G16">
+        <v>1.0701000000000001</v>
+      </c>
+      <c r="H16">
+        <v>1.1327799999999999</v>
+      </c>
+      <c r="I16">
+        <v>1.18068</v>
+      </c>
+      <c r="J16">
+        <v>1.1091299999999999</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>0.03</v>
+      </c>
+      <c r="B17">
+        <v>1.0050600000000001</v>
+      </c>
+      <c r="C17">
+        <v>1.0156099999999999</v>
+      </c>
+      <c r="D17">
+        <v>1.01387</v>
+      </c>
+      <c r="E17">
+        <v>1.04257</v>
+      </c>
+      <c r="F17">
+        <v>1.06674</v>
+      </c>
+      <c r="G17">
+        <v>1.0508299999999999</v>
+      </c>
+      <c r="H17">
+        <v>1.3234300000000001</v>
+      </c>
+      <c r="I17">
+        <v>1.1149500000000001</v>
+      </c>
+      <c r="J17">
+        <v>1.0848199999999999</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>0.02</v>
+      </c>
+      <c r="B18">
+        <v>1.00587</v>
+      </c>
+      <c r="C18">
+        <v>1.0197400000000001</v>
+      </c>
+      <c r="D18">
+        <v>1.0099800000000001</v>
+      </c>
+      <c r="E18">
+        <v>1.0406899999999999</v>
+      </c>
+      <c r="F18">
+        <v>1.0400100000000001</v>
+      </c>
+      <c r="G18">
+        <v>1.0263800000000001</v>
+      </c>
+      <c r="H18">
+        <v>1.1544700000000001</v>
+      </c>
+      <c r="I18">
+        <v>1.09222</v>
+      </c>
+      <c r="J18">
+        <v>1.0683499999999999</v>
+      </c>
+      <c r="K18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0.01</v>
+      </c>
+      <c r="B19">
+        <v>1.0023500000000001</v>
+      </c>
+      <c r="C19">
+        <v>1.00874</v>
+      </c>
+      <c r="D19">
+        <v>1.01675</v>
+      </c>
+      <c r="E19">
+        <v>1.01885</v>
+      </c>
+      <c r="F19">
+        <v>1.0234300000000001</v>
+      </c>
+      <c r="G19">
+        <v>1.01902</v>
+      </c>
+      <c r="H19">
+        <v>1.28898</v>
+      </c>
+      <c r="I19">
+        <v>1.0397400000000001</v>
+      </c>
+      <c r="J19">
+        <v>1.0155700000000001</v>
+      </c>
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:U20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2517,70 +3229,70 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1.9487000000000001</v>
+        <v>1.94872</v>
       </c>
       <c r="C3">
-        <v>4.1204000000000001</v>
+        <v>4.1204799999999997</v>
       </c>
       <c r="D3">
-        <v>6.7554999999999996</v>
+        <v>6.75556</v>
       </c>
       <c r="E3">
-        <v>9.5959000000000003</v>
+        <v>9.5959599999999998</v>
       </c>
       <c r="F3">
-        <v>12.436</v>
+        <v>12.436360000000001</v>
       </c>
       <c r="G3">
-        <v>14.212999999999999</v>
+        <v>14.21374</v>
       </c>
       <c r="H3">
-        <v>16.443999999999999</v>
+        <v>16.44444</v>
       </c>
       <c r="I3">
-        <v>8.5976999999999997</v>
+        <v>8.5977700000000006</v>
       </c>
       <c r="J3">
-        <v>6.7708000000000004</v>
+        <v>6.7708300000000001</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="M3">
         <f>B23/B3</f>
-        <v>0.95122902447785707</v>
+        <v>0.95121926187446126</v>
       </c>
       <c r="N3">
         <f t="shared" ref="N3:U18" si="0">C23/C3</f>
-        <v>0.40078147752645377</v>
+        <v>0.33038383877606492</v>
       </c>
       <c r="O3">
         <f t="shared" si="0"/>
-        <v>0.22639478943083413</v>
+        <v>0.2612233478793764</v>
       </c>
       <c r="P3">
         <f t="shared" si="0"/>
-        <v>0.15789555956189621</v>
+        <v>0.1541575829828386</v>
       </c>
       <c r="Q3">
         <f t="shared" si="0"/>
-        <v>0.15732711482791895</v>
+        <v>0.14006831580944906</v>
       </c>
       <c r="R3">
         <f t="shared" si="0"/>
-        <v>0.11224583128122143</v>
+        <v>0.11223998750504793</v>
       </c>
       <c r="S3">
         <f t="shared" si="0"/>
-        <v>0.10897591826806131</v>
+        <v>0.10897300242513579</v>
       </c>
       <c r="T3">
         <f t="shared" si="0"/>
-        <v>0.20260534794189144</v>
+        <v>0.21170838484862933</v>
       </c>
       <c r="U3">
         <f t="shared" si="0"/>
-        <v>0.316485496543983</v>
+        <v>0.28402426290425248</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -2588,70 +3300,70 @@
         <v>1.8</v>
       </c>
       <c r="B4">
-        <v>1.4396</v>
+        <v>1.45455</v>
       </c>
       <c r="C4">
-        <v>2.3477999999999999</v>
+        <v>2.30769</v>
       </c>
       <c r="D4">
-        <v>4.1120999999999999</v>
+        <v>4.1025600000000004</v>
       </c>
       <c r="E4">
-        <v>4.6595000000000004</v>
+        <v>4.9056600000000001</v>
       </c>
       <c r="F4">
-        <v>7.8387000000000002</v>
+        <v>7.9024400000000004</v>
       </c>
       <c r="G4">
-        <v>8.6068999999999996</v>
+        <v>8.6069600000000008</v>
       </c>
       <c r="H4">
-        <v>24.466000000000001</v>
+        <v>22.665420000000001</v>
       </c>
       <c r="I4">
-        <v>6.0994000000000002</v>
+        <v>6.3679199999999998</v>
       </c>
       <c r="J4">
-        <v>5.3333000000000004</v>
+        <v>6.18893</v>
       </c>
       <c r="L4" s="6">
         <v>1.8</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:U20" si="1">B24/B4</f>
-        <v>0.81403167546540711</v>
+        <v>0.78727441476745386</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>0.5699165175909362</v>
+        <v>0.57452257452257449</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>0.43376620218379902</v>
+        <v>0.40238046488046486</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>0.41034016525378258</v>
+        <v>0.42467884035991083</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>0.26066056871675147</v>
+        <v>0.32666999053456908</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>0.29424996223959848</v>
+        <v>0.27987465957782998</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>0.13124131447723369</v>
+        <v>0.11856343275350732</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>0.74413712824212208</v>
+        <v>0.60117118305506356</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>0.7591134944593404</v>
+        <v>0.64516806620853684</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -2659,70 +3371,70 @@
         <v>1.6</v>
       </c>
       <c r="B5">
-        <v>1.3865000000000001</v>
+        <v>1.4200699999999999</v>
       </c>
       <c r="C5">
-        <v>2.2334999999999998</v>
+        <v>2.23766</v>
       </c>
       <c r="D5">
-        <v>4.1454000000000004</v>
+        <v>4.1931000000000003</v>
       </c>
       <c r="E5">
-        <v>4.6595000000000004</v>
+        <v>4.9056600000000001</v>
       </c>
       <c r="F5">
-        <v>6.8936000000000002</v>
+        <v>6.9428599999999996</v>
       </c>
       <c r="G5">
-        <v>8.5033999999999992</v>
+        <v>8.5034399999999994</v>
       </c>
       <c r="H5">
-        <v>24.417000000000002</v>
+        <v>20.911439999999999</v>
       </c>
       <c r="I5">
-        <v>5.9036999999999997</v>
+        <v>6.2888200000000003</v>
       </c>
       <c r="J5">
-        <v>5.3333000000000004</v>
+        <v>6.18893</v>
       </c>
       <c r="L5" s="6">
         <v>1.6</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>0.815311936530833</v>
+        <v>0.79093988324519215</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>0.59596597268860541</v>
+        <v>0.60069894443302385</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>0.42164809186085778</v>
+        <v>0.39369201783883045</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>0.48647923596952458</v>
+        <v>0.47864507528039035</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>0.28739845653939883</v>
+        <v>0.38457926560524053</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>0.27600254016040648</v>
+        <v>0.29063414335845261</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>0.11058320022934839</v>
+        <v>0.1415110580619986</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>0.44530548638989115</v>
+        <v>0.41215999185856805</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>0.62027825173907325</v>
+        <v>0.48036898139096745</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -2730,70 +3442,70 @@
         <v>1.4</v>
       </c>
       <c r="B6">
-        <v>1.3204</v>
+        <v>1.3141</v>
       </c>
       <c r="C6">
-        <v>2.0535999999999999</v>
+        <v>2.1213199999999999</v>
       </c>
       <c r="D6">
-        <v>2.9779</v>
+        <v>2.97323</v>
       </c>
       <c r="E6">
-        <v>4.6595000000000004</v>
+        <v>4.4142599999999996</v>
       </c>
       <c r="F6">
-        <v>6.2709000000000001</v>
+        <v>6.2207999999999997</v>
       </c>
       <c r="G6">
-        <v>8.5770999999999997</v>
+        <v>8.5771200000000007</v>
       </c>
       <c r="H6">
-        <v>19.803999999999998</v>
+        <v>19.836870000000001</v>
       </c>
       <c r="I6">
-        <v>5.8695000000000004</v>
+        <v>6.25</v>
       </c>
       <c r="J6">
-        <v>5.3333000000000004</v>
+        <v>5.99369</v>
       </c>
       <c r="L6" s="6">
         <v>1.4</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>0.84637231142078162</v>
+        <v>0.85352712883342208</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0.70120763537202957</v>
+        <v>0.64468349895348187</v>
       </c>
       <c r="O6">
         <f t="shared" si="0"/>
-        <v>0.53895026696665438</v>
+        <v>0.6015410849480195</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>0.40807168151089168</v>
+        <v>0.42124840856678131</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>0.26462070835127333</v>
+        <v>0.29375803755144037</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>0.23606930081262897</v>
+        <v>0.31572719047885534</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>0.16208998182185419</v>
+        <v>0.14199770427491837</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>0.64707726382144981</v>
+        <v>0.41248479999999998</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>0.51529634560215998</v>
+        <v>0.62447006768785174</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2801,70 +3513,70 @@
         <v>1.2</v>
       </c>
       <c r="B7">
-        <v>1.2823</v>
+        <v>1.29762</v>
       </c>
       <c r="C7">
-        <v>1.9759</v>
+        <v>1.95652</v>
       </c>
       <c r="D7">
-        <v>2.9937999999999998</v>
+        <v>3.0216699999999999</v>
       </c>
       <c r="E7">
-        <v>4.9470000000000001</v>
+        <v>4.65116</v>
       </c>
       <c r="F7">
-        <v>4.5468999999999999</v>
+        <v>4.5259499999999999</v>
       </c>
       <c r="G7">
-        <v>7.2565999999999997</v>
+        <v>7.0902599999999998</v>
       </c>
       <c r="H7">
-        <v>19.795000000000002</v>
+        <v>19.828060000000001</v>
       </c>
       <c r="I7">
-        <v>4.2901999999999996</v>
+        <v>4.2993600000000001</v>
       </c>
       <c r="J7">
-        <v>5.5921000000000003</v>
+        <v>6.2305299999999999</v>
       </c>
       <c r="L7" s="6">
         <v>1.2</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>0.91321063713639561</v>
+        <v>0.88834943974353053</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0.74911685814059414</v>
+        <v>0.76891623903665685</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>0.63357271694835993</v>
+        <v>0.50956921172728986</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>0.33524964625025266</v>
+        <v>0.33593770156262093</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>0.51918010072796861</v>
+        <v>0.37692639114440063</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>0.29325028250144697</v>
+        <v>0.3011116658627469</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>0.13744733518565291</v>
+        <v>0.14149039290782861</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>0.67483567199664352</v>
+        <v>0.64965483234714005</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>0.5043740276461437</v>
+        <v>0.46007322009524065</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2872,70 +3584,70 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>1.3314999999999999</v>
+        <v>1.34409</v>
       </c>
       <c r="C8">
-        <v>1.7633000000000001</v>
+        <v>1.7769200000000001</v>
       </c>
       <c r="D8">
-        <v>2.8948</v>
+        <v>2.9029500000000001</v>
       </c>
       <c r="E8">
-        <v>4.9470000000000001</v>
+        <v>4.3478300000000001</v>
       </c>
       <c r="F8">
-        <v>4.5568999999999997</v>
+        <v>4.4948899999999998</v>
       </c>
       <c r="G8">
-        <v>6.0011000000000001</v>
+        <v>5.8822799999999997</v>
       </c>
       <c r="H8">
-        <v>19.818999999999999</v>
+        <v>19.851369999999999</v>
       </c>
       <c r="I8">
-        <v>4.609</v>
+        <v>4.6188000000000002</v>
       </c>
       <c r="J8">
-        <v>5.5921000000000003</v>
+        <v>4.9751200000000004</v>
       </c>
       <c r="L8" s="6">
         <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>0.82642883965452496</v>
+        <v>0.85196675817839573</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>0.83412918958770488</v>
+        <v>0.81400963464871801</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0.49744369213762607</v>
+        <v>0.59692726364560189</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>0.3345562967455023</v>
+        <v>0.39958784037094369</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0.40470056397989862</v>
+        <v>0.38658788090476076</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>0.38474612987618934</v>
+        <v>0.40558592926552289</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>0.13576315656693072</v>
+        <v>0.12474453904188981</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>0.64492948578867437</v>
+        <v>0.60869489910799346</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>0.76638650954024423</v>
+        <v>0.61734390326263477</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2943,70 +3655,70 @@
         <v>0.8</v>
       </c>
       <c r="B9">
-        <v>1.2581</v>
+        <v>1.2567699999999999</v>
       </c>
       <c r="C9">
-        <v>1.6596</v>
+        <v>1.64405</v>
       </c>
       <c r="D9">
-        <v>2.9049999999999998</v>
+        <v>2.9497200000000001</v>
       </c>
       <c r="E9">
-        <v>3.3184999999999998</v>
+        <v>3.0927799999999999</v>
       </c>
       <c r="F9">
-        <v>4.4607999999999999</v>
+        <v>4.4657200000000001</v>
       </c>
       <c r="G9">
-        <v>4.4348999999999998</v>
+        <v>4.4466999999999999</v>
       </c>
       <c r="H9">
-        <v>19.504000000000001</v>
+        <v>17.41743</v>
       </c>
       <c r="I9">
-        <v>4.5753000000000004</v>
+        <v>4.5849099999999998</v>
       </c>
       <c r="J9">
-        <v>3.629</v>
+        <v>4.1832700000000003</v>
       </c>
       <c r="L9" s="6">
         <v>0.8</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>0.86679914156267379</v>
+        <v>0.90639496487026272</v>
       </c>
       <c r="N9">
         <f t="shared" si="0"/>
-        <v>0.84643287539166068</v>
+        <v>0.85260180651440043</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>0.53625129087779688</v>
+        <v>0.49708446903434894</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0.4613891818592738</v>
+        <v>0.46710726272156444</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>0.47258563486370159</v>
+        <v>0.35481624463692307</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>0.4031680533946651</v>
+        <v>0.50734027481053368</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0.11534915914684166</v>
+        <v>0.13683362011502273</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>0.57992262802439176</v>
+        <v>0.566641438981354</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>0.91972995315513917</v>
+        <v>0.81113817659390852</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -3014,70 +3726,70 @@
         <v>0.6</v>
       </c>
       <c r="B10">
-        <v>1.1354</v>
+        <v>1.14236</v>
       </c>
       <c r="C10">
-        <v>1.4491000000000001</v>
+        <v>1.42066</v>
       </c>
       <c r="D10">
-        <v>2.0545</v>
+        <v>2.0509200000000001</v>
       </c>
       <c r="E10">
-        <v>3.012</v>
+        <v>2.7198500000000001</v>
       </c>
       <c r="F10">
-        <v>3.5554999999999999</v>
+        <v>3.5036499999999999</v>
       </c>
       <c r="G10">
-        <v>4.2034000000000002</v>
+        <v>4.0930799999999996</v>
       </c>
       <c r="H10">
-        <v>14.205</v>
+        <v>12.900790000000001</v>
       </c>
       <c r="I10">
-        <v>2.8833000000000002</v>
+        <v>2.8038500000000002</v>
       </c>
       <c r="J10">
-        <v>3.629</v>
+        <v>4.1832700000000003</v>
       </c>
       <c r="L10" s="6">
         <v>0.6</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>0.95753038576713057</v>
+        <v>0.92191603347456152</v>
       </c>
       <c r="N10">
         <f t="shared" si="0"/>
-        <v>0.90498240287074727</v>
+        <v>0.91874903213999115</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>0.79676807009004624</v>
+        <v>0.72779045501531014</v>
       </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>0.58708167330677286</v>
+        <v>0.68058900307002224</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
-        <v>0.46097032766136975</v>
+        <v>0.44886903657614208</v>
       </c>
       <c r="R10">
         <f t="shared" si="0"/>
-        <v>0.44663605652566962</v>
+        <v>0.44338493261797968</v>
       </c>
       <c r="S10">
         <f t="shared" si="0"/>
-        <v>0.13887785990848292</v>
+        <v>0.14009917222123605</v>
       </c>
       <c r="T10">
         <f t="shared" si="0"/>
-        <v>0.74964103631255841</v>
+        <v>0.86265313765001694</v>
       </c>
       <c r="U10">
         <f t="shared" si="0"/>
-        <v>0.70703499586662999</v>
+        <v>0.56531373781754468</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -3085,70 +3797,70 @@
         <v>0.4</v>
       </c>
       <c r="B11">
-        <v>1.1023000000000001</v>
+        <v>1.09456</v>
       </c>
       <c r="C11">
-        <v>1.3512999999999999</v>
+        <v>1.3391900000000001</v>
       </c>
       <c r="D11">
-        <v>1.78</v>
+        <v>1.79135</v>
       </c>
       <c r="E11">
-        <v>2.0238</v>
+        <v>2.0833300000000001</v>
       </c>
       <c r="F11">
-        <v>2.7378999999999998</v>
+        <v>2.7275999999999998</v>
       </c>
       <c r="G11">
-        <v>3.3323</v>
+        <v>3.33629</v>
       </c>
       <c r="H11">
-        <v>13.944000000000001</v>
+        <v>11.38686</v>
       </c>
       <c r="I11">
-        <v>2.8125</v>
+        <v>2.8272300000000001</v>
       </c>
       <c r="J11">
-        <v>2.2624</v>
+        <v>2.68065</v>
       </c>
       <c r="L11" s="6">
         <v>0.4</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>1.0000725755239044</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <f t="shared" si="0"/>
-        <v>0.89895656034929339</v>
+        <v>0.89157625131609408</v>
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
-        <v>0.78162921348314607</v>
+        <v>0.7621514500237252</v>
       </c>
       <c r="P11">
         <f t="shared" si="0"/>
-        <v>0.90012847119280559</v>
+        <v>0.85156936251097992</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
-        <v>0.58487161693268575</v>
+        <v>0.6277936647602288</v>
       </c>
       <c r="R11">
         <f t="shared" si="0"/>
-        <v>0.59646790505056568</v>
+        <v>0.5595047193139685</v>
       </c>
       <c r="S11">
         <f t="shared" si="0"/>
-        <v>0.14152467010900743</v>
+        <v>0.13820930440876589</v>
       </c>
       <c r="T11">
         <f t="shared" si="0"/>
-        <v>0.76737422222222229</v>
+        <v>0.60763362018654299</v>
       </c>
       <c r="U11">
         <f t="shared" si="0"/>
-        <v>1.006798090523338</v>
+        <v>0.84217260738999866</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -3156,70 +3868,70 @@
         <v>0.2</v>
       </c>
       <c r="B12">
-        <v>1.0469999999999999</v>
+        <v>1.0562100000000001</v>
       </c>
       <c r="C12">
-        <v>1.1408</v>
+        <v>1.1480999999999999</v>
       </c>
       <c r="D12">
-        <v>1.3358000000000001</v>
+        <v>1.3371599999999999</v>
       </c>
       <c r="E12">
-        <v>1.5462</v>
+        <v>1.56202</v>
       </c>
       <c r="F12">
-        <v>1.6491</v>
+        <v>1.7184299999999999</v>
       </c>
       <c r="G12">
-        <v>2.0402999999999998</v>
+        <v>2.0326200000000001</v>
       </c>
       <c r="H12">
-        <v>8.7086000000000006</v>
+        <v>7.0184600000000001</v>
       </c>
       <c r="I12">
-        <v>1.8224</v>
+        <v>1.84819</v>
       </c>
       <c r="J12">
-        <v>1.7141999999999999</v>
+        <v>1.71723</v>
       </c>
       <c r="L12" s="6">
         <v>0.2</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>1.0131709646609359</v>
+        <v>1</v>
       </c>
       <c r="N12">
         <f t="shared" si="0"/>
-        <v>1.0063990182328189</v>
+        <v>1</v>
       </c>
       <c r="O12">
         <f t="shared" si="0"/>
-        <v>0.8894594999251384</v>
+        <v>0.886071973436238</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
-        <v>0.89404992885784496</v>
+        <v>0.86394540402811737</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
-        <v>0.99564004608574375</v>
+        <v>0.94700977054637081</v>
       </c>
       <c r="R12">
         <f t="shared" si="0"/>
-        <v>0.78933000049012414</v>
+        <v>0.82182109789335922</v>
       </c>
       <c r="S12">
         <f t="shared" si="0"/>
-        <v>0.16273338998231635</v>
+        <v>0.24695730972321564</v>
       </c>
       <c r="T12">
         <f t="shared" si="0"/>
-        <v>0.86871158911325719</v>
+        <v>0.82126296538775767</v>
       </c>
       <c r="U12">
         <f t="shared" si="0"/>
-        <v>0.96364484890911217</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -3227,70 +3939,70 @@
         <v>0.1</v>
       </c>
       <c r="B13">
-        <v>1.0308999999999999</v>
+        <v>1.02349</v>
       </c>
       <c r="C13">
-        <v>1.0445</v>
+        <v>1.0375399999999999</v>
       </c>
       <c r="D13">
-        <v>1.1161000000000001</v>
+        <v>1.1470199999999999</v>
       </c>
       <c r="E13">
-        <v>1.1924999999999999</v>
+        <v>1.2188300000000001</v>
       </c>
       <c r="F13">
-        <v>1.2838000000000001</v>
+        <v>1.2861199999999999</v>
       </c>
       <c r="G13">
-        <v>1.3613</v>
+        <v>1.36744</v>
       </c>
       <c r="H13">
-        <v>4.4134000000000002</v>
+        <v>4.1196099999999998</v>
       </c>
       <c r="I13">
-        <v>1.4151</v>
+        <v>1.3602700000000001</v>
       </c>
       <c r="J13">
-        <v>1.2826</v>
+        <v>1.3713900000000001</v>
       </c>
       <c r="L13" s="6">
         <v>0.1</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>0.9961392957609857</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <f t="shared" si="0"/>
-        <v>0.9958257539492581</v>
+        <v>1</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>1.0296568407848758</v>
+        <v>1</v>
       </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>1.0220796645702308</v>
+        <v>1</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>1.0014877706807912</v>
+        <v>1</v>
       </c>
       <c r="R13">
         <f t="shared" si="0"/>
-        <v>0.97423051494894586</v>
+        <v>0.97670098870882816</v>
       </c>
       <c r="S13">
         <f t="shared" si="0"/>
-        <v>0.26192051479584899</v>
+        <v>0.30461621367071157</v>
       </c>
       <c r="T13">
         <f t="shared" si="0"/>
-        <v>0.88460179492615365</v>
+        <v>0.92414741191087058</v>
       </c>
       <c r="U13">
         <f t="shared" si="0"/>
-        <v>1.0692265710276003</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -3298,70 +4010,70 @@
         <v>0.08</v>
       </c>
       <c r="B14">
-        <v>1.0136000000000001</v>
+        <v>1.0143200000000001</v>
       </c>
       <c r="C14">
-        <v>1.0397000000000001</v>
+        <v>1.0368200000000001</v>
       </c>
       <c r="D14">
-        <v>1.099</v>
+        <v>1.0849800000000001</v>
       </c>
       <c r="E14">
-        <v>1.1931</v>
+        <v>1.1451100000000001</v>
       </c>
       <c r="F14">
-        <v>1.2103999999999999</v>
+        <v>1.20323</v>
       </c>
       <c r="G14">
-        <v>1.2941</v>
+        <v>1.29548</v>
       </c>
       <c r="H14">
-        <v>3.3788</v>
+        <v>3.4682400000000002</v>
       </c>
       <c r="I14">
-        <v>1.3243</v>
+        <v>1.32534</v>
       </c>
       <c r="J14">
-        <v>1.3812</v>
+        <v>1.25722</v>
       </c>
       <c r="L14" s="6">
         <v>0.08</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>1.0015982636148382</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="0"/>
-        <v>0.99824949504664795</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>0.98811646951774335</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="0"/>
-        <v>0.95977705137876124</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>0.99445637805684073</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="0"/>
-        <v>1.0019472992813538</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>0.36463241387474837</v>
+        <v>0.35257940626946233</v>
       </c>
       <c r="T14">
         <f t="shared" si="0"/>
-        <v>0.90665257116967446</v>
+        <v>0.91218857048002777</v>
       </c>
       <c r="U14">
         <f t="shared" si="0"/>
-        <v>0.91023747465971616</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -3369,70 +4081,70 @@
         <v>0.06</v>
       </c>
       <c r="B15">
-        <v>1.0046999999999999</v>
+        <v>1.00759</v>
       </c>
       <c r="C15">
-        <v>1.0316000000000001</v>
+        <v>1.03349</v>
       </c>
       <c r="D15">
-        <v>1.0375000000000001</v>
+        <v>1.0370699999999999</v>
       </c>
       <c r="E15">
-        <v>1.1048</v>
+        <v>1.10328</v>
       </c>
       <c r="F15">
-        <v>1.0867</v>
+        <v>1.0844400000000001</v>
       </c>
       <c r="G15">
-        <v>1.2043999999999999</v>
+        <v>1.2034800000000001</v>
       </c>
       <c r="H15">
-        <v>2.9257</v>
+        <v>2.7916400000000001</v>
       </c>
       <c r="I15">
-        <v>1.2811999999999999</v>
+        <v>1.26431</v>
       </c>
       <c r="J15">
-        <v>1.1007</v>
+        <v>1.1868300000000001</v>
       </c>
       <c r="L15" s="6">
         <v>0.06</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>1.0017219070369265</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
-        <v>1.0023167894532763</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
-        <v>0.99958554216867457</v>
+        <v>1</v>
       </c>
       <c r="P15">
         <f t="shared" si="0"/>
-        <v>0.99862418537291819</v>
+        <v>1</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
-        <v>0.99725775282966778</v>
+        <v>1</v>
       </c>
       <c r="R15">
         <f t="shared" si="0"/>
-        <v>0.99884589837263371</v>
+        <v>1</v>
       </c>
       <c r="S15">
         <f t="shared" si="0"/>
-        <v>0.40260792289024849</v>
+        <v>0.4210679027381754</v>
       </c>
       <c r="T15">
         <f t="shared" si="0"/>
-        <v>0.98719169528566986</v>
+        <v>1</v>
       </c>
       <c r="U15">
         <f t="shared" si="0"/>
-        <v>1.0782502044153721</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -3440,70 +4152,70 @@
         <v>0.05</v>
       </c>
       <c r="B16">
-        <v>1.0195000000000001</v>
+        <v>1.0159199999999999</v>
       </c>
       <c r="C16">
-        <v>1.0253000000000001</v>
+        <v>1.02633</v>
       </c>
       <c r="D16">
-        <v>1.0491999999999999</v>
+        <v>1.0484500000000001</v>
       </c>
       <c r="E16">
-        <v>1.0885</v>
+        <v>1.0731200000000001</v>
       </c>
       <c r="F16">
-        <v>1.0593999999999999</v>
+        <v>1.0606899999999999</v>
       </c>
       <c r="G16">
-        <v>1.1168</v>
+        <v>1.12141</v>
       </c>
       <c r="H16">
-        <v>2.6025999999999998</v>
+        <v>2.5699399999999999</v>
       </c>
       <c r="I16">
-        <v>1.2155</v>
+        <v>1.2327399999999999</v>
       </c>
       <c r="J16">
-        <v>1.1761999999999999</v>
+        <v>1.15544</v>
       </c>
       <c r="L16" s="6">
         <v>0.05</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>0.99838155958803321</v>
+        <v>1</v>
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
-        <v>0.99976592216912119</v>
+        <v>1</v>
       </c>
       <c r="O16">
         <f t="shared" si="0"/>
-        <v>0.99992375142966083</v>
+        <v>1</v>
       </c>
       <c r="P16">
         <f t="shared" si="0"/>
-        <v>0.98618282039503913</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
-        <v>1.0001793468000757</v>
+        <v>1</v>
       </c>
       <c r="R16">
         <f t="shared" si="0"/>
-        <v>1.0057664756446991</v>
+        <v>1</v>
       </c>
       <c r="S16">
         <f t="shared" si="0"/>
-        <v>0.45604395604395609</v>
+        <v>0.44670692700996911</v>
       </c>
       <c r="T16">
         <f t="shared" si="0"/>
-        <v>1.0146770876182643</v>
+        <v>1</v>
       </c>
       <c r="U16">
         <f t="shared" si="0"/>
-        <v>0.98234994048631197</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -3511,70 +4223,70 @@
         <v>0.04</v>
       </c>
       <c r="B17">
-        <v>1.004</v>
+        <v>1.0027699999999999</v>
       </c>
       <c r="C17">
-        <v>1.0185</v>
+        <v>1.02755</v>
       </c>
       <c r="D17">
-        <v>1.0021</v>
+        <v>1.00502</v>
       </c>
       <c r="E17">
-        <v>1.0607</v>
+        <v>1.05935</v>
       </c>
       <c r="F17">
-        <v>1.0738000000000001</v>
+        <v>1.0763400000000001</v>
       </c>
       <c r="G17">
-        <v>1.0725</v>
+        <v>1.0701000000000001</v>
       </c>
       <c r="H17">
-        <v>2.2029999999999998</v>
+        <v>2.2174299999999998</v>
       </c>
       <c r="I17">
-        <v>1.1715</v>
+        <v>1.18068</v>
       </c>
       <c r="J17">
-        <v>1.171</v>
+        <v>1.1091299999999999</v>
       </c>
       <c r="L17" s="6">
         <v>0.04</v>
       </c>
       <c r="M17">
         <f t="shared" si="1"/>
-        <v>0.99774900398406385</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>1.0081001472754052</v>
+        <v>1</v>
       </c>
       <c r="O17">
         <f t="shared" si="0"/>
-        <v>1.0041911984831853</v>
+        <v>1</v>
       </c>
       <c r="P17">
         <f t="shared" si="0"/>
-        <v>0.99872725558593389</v>
+        <v>1</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
-        <v>1.0016017880424659</v>
+        <v>1</v>
       </c>
       <c r="R17">
         <f t="shared" si="0"/>
-        <v>0.99764102564102575</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <f t="shared" si="0"/>
-        <v>0.51006354970494783</v>
+        <v>0.51085265374780719</v>
       </c>
       <c r="T17">
         <f t="shared" si="0"/>
-        <v>1.0064020486555698</v>
+        <v>1</v>
       </c>
       <c r="U17">
         <f t="shared" si="0"/>
-        <v>0.9471648163962425</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -3582,70 +4294,70 @@
         <v>0.03</v>
       </c>
       <c r="B18">
-        <v>1.0048999999999999</v>
+        <v>1.0050600000000001</v>
       </c>
       <c r="C18">
-        <v>1.0141</v>
+        <v>1.0156099999999999</v>
       </c>
       <c r="D18">
-        <v>1.0212000000000001</v>
+        <v>1.01387</v>
       </c>
       <c r="E18">
-        <v>1.0452999999999999</v>
+        <v>1.04257</v>
       </c>
       <c r="F18">
-        <v>1.0598000000000001</v>
+        <v>1.06674</v>
       </c>
       <c r="G18">
-        <v>1.0502</v>
+        <v>1.0508299999999999</v>
       </c>
       <c r="H18">
-        <v>1.9265000000000001</v>
+        <v>1.8624400000000001</v>
       </c>
       <c r="I18">
-        <v>1.1009</v>
+        <v>1.1149500000000001</v>
       </c>
       <c r="J18">
-        <v>1.0412999999999999</v>
+        <v>1.0848199999999999</v>
       </c>
       <c r="L18" s="6">
         <v>0.03</v>
       </c>
       <c r="M18">
         <f t="shared" si="1"/>
-        <v>1.0005473181411086</v>
+        <v>1</v>
       </c>
       <c r="N18">
         <f t="shared" si="0"/>
-        <v>1.0008579035598066</v>
+        <v>1</v>
       </c>
       <c r="O18">
         <f t="shared" si="0"/>
-        <v>0.99296905601253405</v>
+        <v>1</v>
       </c>
       <c r="P18">
         <f t="shared" si="0"/>
-        <v>0.99738830957619828</v>
+        <v>1</v>
       </c>
       <c r="Q18">
         <f t="shared" si="0"/>
-        <v>1.0061615399131911</v>
+        <v>1</v>
       </c>
       <c r="R18">
         <f t="shared" si="0"/>
-        <v>1.0012569034469625</v>
+        <v>1</v>
       </c>
       <c r="S18">
         <f t="shared" si="0"/>
-        <v>0.68279262912016603</v>
+        <v>0.71058933442151162</v>
       </c>
       <c r="T18">
         <f t="shared" si="0"/>
-        <v>1.0131982923062948</v>
+        <v>1</v>
       </c>
       <c r="U18">
         <f t="shared" si="0"/>
-        <v>1.0417939114568329</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -3653,70 +4365,70 @@
         <v>0.02</v>
       </c>
       <c r="B19">
-        <v>1.0065</v>
+        <v>1.00587</v>
       </c>
       <c r="C19">
-        <v>1.0159</v>
+        <v>1.0197400000000001</v>
       </c>
       <c r="D19">
-        <v>1.0087999999999999</v>
+        <v>1.0099800000000001</v>
       </c>
       <c r="E19">
-        <v>1.0337000000000001</v>
+        <v>1.0406899999999999</v>
       </c>
       <c r="F19">
-        <v>1.0216000000000001</v>
+        <v>1.0400100000000001</v>
       </c>
       <c r="G19">
-        <v>1.0239</v>
+        <v>1.0263800000000001</v>
       </c>
       <c r="H19">
-        <v>1.5729</v>
+        <v>1.5659700000000001</v>
       </c>
       <c r="I19">
-        <v>1.0811999999999999</v>
+        <v>1.09222</v>
       </c>
       <c r="J19">
-        <v>1.0966</v>
+        <v>1.0683499999999999</v>
       </c>
       <c r="L19" s="6">
         <v>0.02</v>
       </c>
       <c r="M19">
         <f t="shared" si="1"/>
-        <v>0.99979135618479875</v>
+        <v>1</v>
       </c>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>1.0034550644748499</v>
+        <v>1</v>
       </c>
       <c r="O19">
         <f t="shared" si="1"/>
-        <v>1.0019131641554322</v>
+        <v>1</v>
       </c>
       <c r="P19">
         <f t="shared" si="1"/>
-        <v>1.0067621166682788</v>
+        <v>1</v>
       </c>
       <c r="Q19">
         <f t="shared" si="1"/>
-        <v>1.0180501174628034</v>
+        <v>1</v>
       </c>
       <c r="R19">
         <f t="shared" si="1"/>
-        <v>1.0019337825959564</v>
+        <v>1</v>
       </c>
       <c r="S19">
         <f t="shared" si="1"/>
-        <v>0.73466208913471942</v>
+        <v>0.73722357388711157</v>
       </c>
       <c r="T19">
         <f t="shared" si="1"/>
-        <v>1.0097299297077322</v>
+        <v>1</v>
       </c>
       <c r="U19">
         <f t="shared" si="1"/>
-        <v>0.97423855553529082</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -3724,677 +4436,677 @@
         <v>0.01</v>
       </c>
       <c r="B20">
-        <v>1.0031000000000001</v>
+        <v>1.0023500000000001</v>
       </c>
       <c r="C20">
-        <v>1.0102</v>
+        <v>1.00874</v>
       </c>
       <c r="D20">
-        <v>1.0081</v>
+        <v>1.01675</v>
       </c>
       <c r="E20">
-        <v>1.0092000000000001</v>
+        <v>1.01885</v>
       </c>
       <c r="F20">
-        <v>1.0382</v>
+        <v>1.0234300000000001</v>
       </c>
       <c r="G20">
-        <v>1.018</v>
+        <v>1.01902</v>
       </c>
       <c r="H20">
-        <v>1.2764</v>
+        <v>1.28898</v>
       </c>
       <c r="I20">
-        <v>1.0432999999999999</v>
+        <v>1.0397400000000001</v>
       </c>
       <c r="J20">
-        <v>1.0218</v>
+        <v>1.0155700000000001</v>
       </c>
       <c r="L20" s="6">
         <v>0.01</v>
       </c>
       <c r="M20">
         <f t="shared" si="1"/>
-        <v>0.99947163792244031</v>
+        <v>1</v>
       </c>
       <c r="N20">
         <f t="shared" si="1"/>
-        <v>0.99858443872500491</v>
+        <v>1</v>
       </c>
       <c r="O20">
         <f t="shared" si="1"/>
-        <v>1.0082233905366531</v>
+        <v>1</v>
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>1.0095917558462146</v>
+        <v>1</v>
       </c>
       <c r="Q20">
         <f t="shared" si="1"/>
-        <v>0.98527258717010202</v>
+        <v>1</v>
       </c>
       <c r="R20">
         <f t="shared" si="1"/>
-        <v>1.0011001964636543</v>
+        <v>1</v>
       </c>
       <c r="S20">
         <f t="shared" si="1"/>
-        <v>1.010294578502037</v>
+        <v>1</v>
       </c>
       <c r="T20">
         <f t="shared" si="1"/>
-        <v>0.99644397584587374</v>
+        <v>1</v>
       </c>
       <c r="U20">
         <f t="shared" si="1"/>
-        <v>0.99390291642200046</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="H22" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>2</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23">
         <v>1.8536600000000001</v>
       </c>
-      <c r="C23" s="7">
-        <v>1.6513800000000001</v>
-      </c>
-      <c r="D23" s="7">
-        <v>1.5294099999999999</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1.51515</v>
-      </c>
-      <c r="F23" s="7">
-        <v>1.95652</v>
-      </c>
-      <c r="G23" s="7">
+      <c r="C23">
+        <v>1.36134</v>
+      </c>
+      <c r="D23">
+        <v>1.76471</v>
+      </c>
+      <c r="E23">
+        <v>1.47929</v>
+      </c>
+      <c r="F23">
+        <v>1.74194</v>
+      </c>
+      <c r="G23">
         <v>1.59535</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23">
         <v>1.792</v>
       </c>
-      <c r="I23" s="7">
-        <v>1.74194</v>
-      </c>
-      <c r="J23" s="7">
-        <v>2.1428600000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
+      <c r="I23">
+        <v>1.8202199999999999</v>
+      </c>
+      <c r="J23">
+        <v>1.9230799999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
         <v>1.8</v>
       </c>
-      <c r="B24" s="7">
-        <v>1.17188</v>
-      </c>
-      <c r="C24" s="7">
-        <v>1.33805</v>
-      </c>
-      <c r="D24" s="7">
-        <v>1.78369</v>
-      </c>
-      <c r="E24" s="7">
-        <v>1.91198</v>
-      </c>
-      <c r="F24" s="7">
-        <v>2.0432399999999999</v>
-      </c>
-      <c r="G24" s="7">
-        <v>2.5325799999999998</v>
-      </c>
-      <c r="H24" s="7">
-        <v>3.21095</v>
-      </c>
-      <c r="I24" s="7">
-        <v>4.5387899999999997</v>
-      </c>
-      <c r="J24" s="7">
-        <v>4.0485800000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
+      <c r="B24">
+        <v>1.14513</v>
+      </c>
+      <c r="C24">
+        <v>1.32582</v>
+      </c>
+      <c r="D24">
+        <v>1.65079</v>
+      </c>
+      <c r="E24">
+        <v>2.0833300000000001</v>
+      </c>
+      <c r="F24">
+        <v>2.5814900000000001</v>
+      </c>
+      <c r="G24">
+        <v>2.4088699999999998</v>
+      </c>
+      <c r="H24">
+        <v>2.68729</v>
+      </c>
+      <c r="I24">
+        <v>3.8282099999999999</v>
+      </c>
+      <c r="J24">
+        <v>3.9929000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
         <v>1.6</v>
       </c>
-      <c r="B25" s="7">
-        <v>1.13043</v>
-      </c>
-      <c r="C25" s="7">
-        <v>1.3310900000000001</v>
-      </c>
-      <c r="D25" s="7">
-        <v>1.7479</v>
-      </c>
-      <c r="E25" s="7">
-        <v>2.26675</v>
-      </c>
-      <c r="F25" s="7">
-        <v>1.9812099999999999</v>
-      </c>
-      <c r="G25" s="7">
-        <v>2.3469600000000002</v>
-      </c>
-      <c r="H25" s="7">
-        <v>2.70011</v>
-      </c>
-      <c r="I25" s="7">
-        <v>2.6289500000000001</v>
-      </c>
-      <c r="J25" s="7">
-        <v>3.3081299999999998</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+      <c r="B25">
+        <v>1.1231899999999999</v>
+      </c>
+      <c r="C25">
+        <v>1.34416</v>
+      </c>
+      <c r="D25">
+        <v>1.65079</v>
+      </c>
+      <c r="E25">
+        <v>2.3480699999999999</v>
+      </c>
+      <c r="F25">
+        <v>2.67008</v>
+      </c>
+      <c r="G25">
+        <v>2.47139</v>
+      </c>
+      <c r="H25">
+        <v>2.9592000000000001</v>
+      </c>
+      <c r="I25">
+        <v>2.5920000000000001</v>
+      </c>
+      <c r="J25">
+        <v>2.9729700000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
         <v>1.4</v>
       </c>
-      <c r="B26" s="7">
-        <v>1.11755</v>
-      </c>
-      <c r="C26" s="7">
-        <v>1.44</v>
-      </c>
-      <c r="D26" s="7">
-        <v>1.60494</v>
-      </c>
-      <c r="E26" s="7">
-        <v>1.90141</v>
-      </c>
-      <c r="F26" s="7">
-        <v>1.6594100000000001</v>
-      </c>
-      <c r="G26" s="7">
-        <v>2.0247899999999999</v>
-      </c>
-      <c r="H26" s="7">
-        <v>3.2100300000000002</v>
-      </c>
-      <c r="I26" s="7">
-        <v>3.7980200000000002</v>
-      </c>
-      <c r="J26" s="7">
-        <v>2.74823</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="B26">
+        <v>1.1216200000000001</v>
+      </c>
+      <c r="C26">
+        <v>1.36758</v>
+      </c>
+      <c r="D26">
+        <v>1.7885200000000001</v>
+      </c>
+      <c r="E26">
+        <v>1.8594999999999999</v>
+      </c>
+      <c r="F26">
+        <v>1.82741</v>
+      </c>
+      <c r="G26">
+        <v>2.7080299999999999</v>
+      </c>
+      <c r="H26">
+        <v>2.8167900000000001</v>
+      </c>
+      <c r="I26">
+        <v>2.57803</v>
+      </c>
+      <c r="J26">
+        <v>3.74288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
         <v>1.2</v>
       </c>
-      <c r="B27" s="7">
-        <v>1.1710100000000001</v>
-      </c>
-      <c r="C27" s="7">
-        <v>1.4801800000000001</v>
-      </c>
-      <c r="D27" s="7">
-        <v>1.89679</v>
-      </c>
-      <c r="E27" s="7">
-        <v>1.65848</v>
-      </c>
-      <c r="F27" s="7">
-        <v>2.3606600000000002</v>
-      </c>
-      <c r="G27" s="7">
-        <v>2.1280000000000001</v>
-      </c>
-      <c r="H27" s="7">
-        <v>2.7207699999999999</v>
-      </c>
-      <c r="I27" s="7">
-        <v>2.8951799999999999</v>
-      </c>
-      <c r="J27" s="7">
-        <v>2.8205100000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>1</v>
-      </c>
-      <c r="B28" s="7">
-        <v>1.10039</v>
-      </c>
-      <c r="C28" s="7">
-        <v>1.47082</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1.44</v>
-      </c>
-      <c r="E28" s="7">
-        <v>1.6550499999999999</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1.8441799999999999</v>
-      </c>
-      <c r="G28" s="7">
-        <v>2.3089</v>
-      </c>
-      <c r="H28" s="7">
-        <v>2.69069</v>
-      </c>
-      <c r="I28" s="7">
-        <v>2.97248</v>
-      </c>
-      <c r="J28" s="7">
-        <v>4.2857099999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A29" s="8">
+      <c r="B27">
+        <v>1.1527400000000001</v>
+      </c>
+      <c r="C27">
+        <v>1.5044</v>
+      </c>
+      <c r="D27">
+        <v>1.53975</v>
+      </c>
+      <c r="E27">
+        <v>1.5625</v>
+      </c>
+      <c r="F27">
+        <v>1.7059500000000001</v>
+      </c>
+      <c r="G27">
+        <v>2.13496</v>
+      </c>
+      <c r="H27">
+        <v>2.8054800000000002</v>
+      </c>
+      <c r="I27">
+        <v>2.7930999999999999</v>
+      </c>
+      <c r="J27">
+        <v>2.8664999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>1.1451199999999999</v>
+      </c>
+      <c r="C28">
+        <v>1.4464300000000001</v>
+      </c>
+      <c r="D28">
+        <v>1.73285</v>
+      </c>
+      <c r="E28">
+        <v>1.7373400000000001</v>
+      </c>
+      <c r="F28">
+        <v>1.73767</v>
+      </c>
+      <c r="G28">
+        <v>2.3857699999999999</v>
+      </c>
+      <c r="H28">
+        <v>2.4763500000000001</v>
+      </c>
+      <c r="I28">
+        <v>2.8114400000000002</v>
+      </c>
+      <c r="J28">
+        <v>3.0713599999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
         <v>0.8</v>
       </c>
-      <c r="B29" s="7">
-        <v>1.0905199999999999</v>
-      </c>
-      <c r="C29" s="7">
-        <v>1.4047400000000001</v>
-      </c>
-      <c r="D29" s="7">
-        <v>1.5578099999999999</v>
-      </c>
-      <c r="E29" s="7">
-        <v>1.53112</v>
-      </c>
-      <c r="F29" s="7">
-        <v>2.1081099999999999</v>
-      </c>
-      <c r="G29" s="7">
-        <v>1.7880100000000001</v>
-      </c>
-      <c r="H29" s="7">
-        <v>2.2497699999999998</v>
-      </c>
-      <c r="I29" s="7">
-        <v>2.6533199999999999</v>
-      </c>
-      <c r="J29" s="7">
-        <v>3.3376999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="B29">
+        <v>1.13913</v>
+      </c>
+      <c r="C29">
+        <v>1.4017200000000001</v>
+      </c>
+      <c r="D29">
+        <v>1.4662599999999999</v>
+      </c>
+      <c r="E29">
+        <v>1.4446600000000001</v>
+      </c>
+      <c r="F29">
+        <v>1.5845100000000001</v>
+      </c>
+      <c r="G29">
+        <v>2.2559900000000002</v>
+      </c>
+      <c r="H29">
+        <v>2.3832900000000001</v>
+      </c>
+      <c r="I29">
+        <v>2.5979999999999999</v>
+      </c>
+      <c r="J29">
+        <v>3.3932099999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
         <v>0.6</v>
       </c>
-      <c r="B30" s="7">
-        <v>1.08718</v>
-      </c>
-      <c r="C30" s="7">
-        <v>1.31141</v>
-      </c>
-      <c r="D30" s="7">
-        <v>1.63696</v>
-      </c>
-      <c r="E30" s="7">
-        <v>1.7682899999999999</v>
-      </c>
-      <c r="F30" s="7">
-        <v>1.6389800000000001</v>
-      </c>
-      <c r="G30" s="7">
-        <v>1.8773899999999999</v>
-      </c>
-      <c r="H30" s="7">
-        <v>1.9727600000000001</v>
-      </c>
-      <c r="I30" s="7">
-        <v>2.1614399999999998</v>
-      </c>
-      <c r="J30" s="7">
-        <v>2.5658300000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="B30">
+        <v>1.0531600000000001</v>
+      </c>
+      <c r="C30">
+        <v>1.3052299999999999</v>
+      </c>
+      <c r="D30">
+        <v>1.49264</v>
+      </c>
+      <c r="E30">
+        <v>1.8511</v>
+      </c>
+      <c r="F30">
+        <v>1.5726800000000001</v>
+      </c>
+      <c r="G30">
+        <v>1.81481</v>
+      </c>
+      <c r="H30">
+        <v>1.8073900000000001</v>
+      </c>
+      <c r="I30">
+        <v>2.4187500000000002</v>
+      </c>
+      <c r="J30">
+        <v>2.3648600000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
         <v>0.4</v>
       </c>
-      <c r="B31" s="7">
-        <v>1.1023799999999999</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1.2147600000000001</v>
-      </c>
-      <c r="D31" s="7">
-        <v>1.3913</v>
-      </c>
-      <c r="E31" s="7">
-        <v>1.82168</v>
-      </c>
-      <c r="F31" s="7">
-        <v>1.6013200000000001</v>
-      </c>
-      <c r="G31" s="7">
-        <v>1.9876100000000001</v>
-      </c>
-      <c r="H31" s="7">
-        <v>1.97342</v>
-      </c>
-      <c r="I31" s="7">
-        <v>2.1582400000000002</v>
-      </c>
-      <c r="J31" s="7">
-        <v>2.2777799999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="B31">
+        <v>1.09456</v>
+      </c>
+      <c r="C31">
+        <v>1.1939900000000001</v>
+      </c>
+      <c r="D31">
+        <v>1.36528</v>
+      </c>
+      <c r="E31">
+        <v>1.7741</v>
+      </c>
+      <c r="F31">
+        <v>1.7123699999999999</v>
+      </c>
+      <c r="G31">
+        <v>1.8666700000000001</v>
+      </c>
+      <c r="H31">
+        <v>1.5737699999999999</v>
+      </c>
+      <c r="I31">
+        <v>1.7179199999999999</v>
+      </c>
+      <c r="J31">
+        <v>2.2575699999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
         <v>0.2</v>
       </c>
-      <c r="B32" s="7">
-        <v>1.0607899999999999</v>
-      </c>
-      <c r="C32" s="7">
+      <c r="B32">
+        <v>1.0562100000000001</v>
+      </c>
+      <c r="C32">
         <v>1.1480999999999999</v>
       </c>
-      <c r="D32" s="7">
-        <v>1.18814</v>
-      </c>
-      <c r="E32" s="7">
-        <v>1.3823799999999999</v>
-      </c>
-      <c r="F32" s="7">
-        <v>1.64191</v>
-      </c>
-      <c r="G32" s="7">
-        <v>1.6104700000000001</v>
-      </c>
-      <c r="H32" s="7">
-        <v>1.4171800000000001</v>
-      </c>
-      <c r="I32" s="7">
-        <v>1.58314</v>
-      </c>
-      <c r="J32" s="7">
-        <v>1.65188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="D32">
+        <v>1.18482</v>
+      </c>
+      <c r="E32">
+        <v>1.3494999999999999</v>
+      </c>
+      <c r="F32">
+        <v>1.62737</v>
+      </c>
+      <c r="G32">
+        <v>1.67045</v>
+      </c>
+      <c r="H32">
+        <v>1.73326</v>
+      </c>
+      <c r="I32">
+        <v>1.5178499999999999</v>
+      </c>
+      <c r="J32">
+        <v>1.71723</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
         <v>0.1</v>
       </c>
-      <c r="B33" s="7">
-        <v>1.0269200000000001</v>
-      </c>
-      <c r="C33" s="7">
-        <v>1.0401400000000001</v>
-      </c>
-      <c r="D33" s="7">
-        <v>1.1492</v>
-      </c>
-      <c r="E33" s="7">
+      <c r="B33">
+        <v>1.02349</v>
+      </c>
+      <c r="C33">
+        <v>1.0375399999999999</v>
+      </c>
+      <c r="D33">
+        <v>1.1470199999999999</v>
+      </c>
+      <c r="E33">
         <v>1.2188300000000001</v>
       </c>
-      <c r="F33" s="7">
-        <v>1.2857099999999999</v>
-      </c>
-      <c r="G33" s="7">
-        <v>1.32622</v>
-      </c>
-      <c r="H33" s="7">
-        <v>1.1559600000000001</v>
-      </c>
-      <c r="I33" s="7">
-        <v>1.2518</v>
-      </c>
-      <c r="J33" s="7">
+      <c r="F33">
+        <v>1.2861199999999999</v>
+      </c>
+      <c r="G33">
+        <v>1.33558</v>
+      </c>
+      <c r="H33">
+        <v>1.2548999999999999</v>
+      </c>
+      <c r="I33">
+        <v>1.25709</v>
+      </c>
+      <c r="J33">
         <v>1.3713900000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="8">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
         <v>0.08</v>
       </c>
-      <c r="B34" s="7">
-        <v>1.01522</v>
-      </c>
-      <c r="C34" s="7">
-        <v>1.0378799999999999</v>
-      </c>
-      <c r="D34" s="7">
-        <v>1.0859399999999999</v>
-      </c>
-      <c r="E34" s="7">
+      <c r="B34">
+        <v>1.0143200000000001</v>
+      </c>
+      <c r="C34">
+        <v>1.0368200000000001</v>
+      </c>
+      <c r="D34">
+        <v>1.0849800000000001</v>
+      </c>
+      <c r="E34">
         <v>1.1451100000000001</v>
       </c>
-      <c r="F34" s="7">
-        <v>1.2036899999999999</v>
-      </c>
-      <c r="G34" s="7">
-        <v>1.2966200000000001</v>
-      </c>
-      <c r="H34" s="7">
-        <v>1.2320199999999999</v>
-      </c>
-      <c r="I34" s="7">
-        <v>1.20068</v>
-      </c>
-      <c r="J34" s="7">
+      <c r="F34">
+        <v>1.20323</v>
+      </c>
+      <c r="G34">
+        <v>1.29548</v>
+      </c>
+      <c r="H34">
+        <v>1.2228300000000001</v>
+      </c>
+      <c r="I34">
+        <v>1.20896</v>
+      </c>
+      <c r="J34">
         <v>1.25722</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="8">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
         <v>0.06</v>
       </c>
-      <c r="B35" s="7">
-        <v>1.0064299999999999</v>
-      </c>
-      <c r="C35" s="7">
-        <v>1.03399</v>
-      </c>
-      <c r="D35" s="7">
+      <c r="B35">
+        <v>1.00759</v>
+      </c>
+      <c r="C35">
+        <v>1.03349</v>
+      </c>
+      <c r="D35">
         <v>1.0370699999999999</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35">
         <v>1.10328</v>
       </c>
-      <c r="F35" s="7">
-        <v>1.08372</v>
-      </c>
-      <c r="G35" s="7">
-        <v>1.2030099999999999</v>
-      </c>
-      <c r="H35" s="7">
-        <v>1.17791</v>
-      </c>
-      <c r="I35" s="7">
-        <v>1.2647900000000001</v>
-      </c>
-      <c r="J35" s="7">
+      <c r="F35">
+        <v>1.0844400000000001</v>
+      </c>
+      <c r="G35">
+        <v>1.2034800000000001</v>
+      </c>
+      <c r="H35">
+        <v>1.17547</v>
+      </c>
+      <c r="I35">
+        <v>1.26431</v>
+      </c>
+      <c r="J35">
         <v>1.1868300000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
         <v>0.05</v>
       </c>
-      <c r="B36" s="7">
-        <v>1.0178499999999999</v>
-      </c>
-      <c r="C36" s="7">
-        <v>1.0250600000000001</v>
-      </c>
-      <c r="D36" s="7">
-        <v>1.0491200000000001</v>
-      </c>
-      <c r="E36" s="7">
-        <v>1.0734600000000001</v>
-      </c>
-      <c r="F36" s="7">
-        <v>1.05959</v>
-      </c>
-      <c r="G36" s="7">
-        <v>1.12324</v>
-      </c>
-      <c r="H36" s="7">
-        <v>1.1869000000000001</v>
-      </c>
-      <c r="I36" s="7">
-        <v>1.2333400000000001</v>
-      </c>
-      <c r="J36" s="7">
+      <c r="B36">
+        <v>1.0159199999999999</v>
+      </c>
+      <c r="C36">
+        <v>1.02633</v>
+      </c>
+      <c r="D36">
+        <v>1.0484500000000001</v>
+      </c>
+      <c r="E36">
+        <v>1.0731200000000001</v>
+      </c>
+      <c r="F36">
+        <v>1.0606899999999999</v>
+      </c>
+      <c r="G36">
+        <v>1.12141</v>
+      </c>
+      <c r="H36">
+        <v>1.14801</v>
+      </c>
+      <c r="I36">
+        <v>1.2327399999999999</v>
+      </c>
+      <c r="J36">
         <v>1.15544</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="8">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
         <v>0.04</v>
       </c>
-      <c r="B37" s="7">
-        <v>1.0017400000000001</v>
-      </c>
-      <c r="C37" s="7">
-        <v>1.0267500000000001</v>
-      </c>
-      <c r="D37" s="7">
-        <v>1.0063</v>
-      </c>
-      <c r="E37" s="7">
+      <c r="B37">
+        <v>1.0027699999999999</v>
+      </c>
+      <c r="C37">
+        <v>1.02755</v>
+      </c>
+      <c r="D37">
+        <v>1.00502</v>
+      </c>
+      <c r="E37">
         <v>1.05935</v>
       </c>
-      <c r="F37" s="7">
-        <v>1.07552</v>
-      </c>
-      <c r="G37" s="7">
-        <v>1.0699700000000001</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1.1236699999999999</v>
-      </c>
-      <c r="I37" s="7">
-        <v>1.179</v>
-      </c>
-      <c r="J37" s="7">
+      <c r="F37">
+        <v>1.0763400000000001</v>
+      </c>
+      <c r="G37">
+        <v>1.0701000000000001</v>
+      </c>
+      <c r="H37">
+        <v>1.1327799999999999</v>
+      </c>
+      <c r="I37">
+        <v>1.18068</v>
+      </c>
+      <c r="J37">
         <v>1.1091299999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="8">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
         <v>0.03</v>
       </c>
-      <c r="B38" s="7">
-        <v>1.00545</v>
-      </c>
-      <c r="C38" s="7">
-        <v>1.0149699999999999</v>
-      </c>
-      <c r="D38" s="7">
-        <v>1.0140199999999999</v>
-      </c>
-      <c r="E38" s="7">
+      <c r="B38">
+        <v>1.0050600000000001</v>
+      </c>
+      <c r="C38">
+        <v>1.0156099999999999</v>
+      </c>
+      <c r="D38">
+        <v>1.01387</v>
+      </c>
+      <c r="E38">
         <v>1.04257</v>
       </c>
-      <c r="F38" s="7">
-        <v>1.06633</v>
-      </c>
-      <c r="G38" s="7">
-        <v>1.05152</v>
-      </c>
-      <c r="H38" s="7">
-        <v>1.3153999999999999</v>
-      </c>
-      <c r="I38" s="7">
-        <v>1.1154299999999999</v>
-      </c>
-      <c r="J38" s="7">
+      <c r="F38">
+        <v>1.06674</v>
+      </c>
+      <c r="G38">
+        <v>1.0508299999999999</v>
+      </c>
+      <c r="H38">
+        <v>1.3234300000000001</v>
+      </c>
+      <c r="I38">
+        <v>1.1149500000000001</v>
+      </c>
+      <c r="J38">
         <v>1.0848199999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="8">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
         <v>0.02</v>
       </c>
-      <c r="B39" s="7">
-        <v>1.0062899999999999</v>
-      </c>
-      <c r="C39" s="7">
-        <v>1.0194099999999999</v>
-      </c>
-      <c r="D39" s="7">
-        <v>1.0107299999999999</v>
-      </c>
-      <c r="E39" s="7">
+      <c r="B39">
+        <v>1.00587</v>
+      </c>
+      <c r="C39">
+        <v>1.0197400000000001</v>
+      </c>
+      <c r="D39">
+        <v>1.0099800000000001</v>
+      </c>
+      <c r="E39">
         <v>1.0406899999999999</v>
       </c>
-      <c r="F39" s="7">
-        <v>1.0400400000000001</v>
-      </c>
-      <c r="G39" s="7">
-        <v>1.0258799999999999</v>
-      </c>
-      <c r="H39" s="7">
-        <v>1.1555500000000001</v>
-      </c>
-      <c r="I39" s="7">
-        <v>1.09172</v>
-      </c>
-      <c r="J39" s="7">
+      <c r="F39">
+        <v>1.0400100000000001</v>
+      </c>
+      <c r="G39">
+        <v>1.0263800000000001</v>
+      </c>
+      <c r="H39">
+        <v>1.1544700000000001</v>
+      </c>
+      <c r="I39">
+        <v>1.09222</v>
+      </c>
+      <c r="J39">
         <v>1.0683499999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="8">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
         <v>0.01</v>
       </c>
-      <c r="B40" s="7">
-        <v>1.00257</v>
-      </c>
-      <c r="C40" s="7">
-        <v>1.0087699999999999</v>
-      </c>
-      <c r="D40" s="7">
-        <v>1.0163899999999999</v>
-      </c>
-      <c r="E40" s="7">
-        <v>1.01888</v>
-      </c>
-      <c r="F40" s="7">
-        <v>1.02291</v>
-      </c>
-      <c r="G40" s="7">
-        <v>1.01912</v>
-      </c>
-      <c r="H40" s="7">
-        <v>1.2895399999999999</v>
-      </c>
-      <c r="I40" s="7">
-        <v>1.03959</v>
-      </c>
-      <c r="J40" s="7">
+      <c r="B40">
+        <v>1.0023500000000001</v>
+      </c>
+      <c r="C40">
+        <v>1.00874</v>
+      </c>
+      <c r="D40">
+        <v>1.01675</v>
+      </c>
+      <c r="E40">
+        <v>1.01885</v>
+      </c>
+      <c r="F40">
+        <v>1.0234300000000001</v>
+      </c>
+      <c r="G40">
+        <v>1.01902</v>
+      </c>
+      <c r="H40">
+        <v>1.28898</v>
+      </c>
+      <c r="I40">
+        <v>1.0397400000000001</v>
+      </c>
+      <c r="J40">
         <v>1.0155700000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More images and text added.
</commit_message>
<xml_diff>
--- a/MetricConvergence.xlsx
+++ b/MetricConvergence.xlsx
@@ -9,16 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6080" yWindow="3820" windowWidth="24740" windowHeight="19500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1340" yWindow="12040" windowWidth="26720" windowHeight="13800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Opposite Pins" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Same Side Pins" sheetId="2" r:id="rId3"/>
+    <sheet name="Same Side Pins" sheetId="2" r:id="rId2"/>
+    <sheet name="Lattice" sheetId="5" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="for_spreadsheet" localSheetId="1">Sheet2!$A$1:$K$19</definedName>
-  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -28,30 +25,8 @@
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="for_spreadsheet" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Volumes/tghaddar/PDTCurrent/restapl-pdt/pdt/inputs/ConvergenceInputs/for_spreadsheet.csv" comma="1">
-      <textFields count="11">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="13">
   <si>
     <t>Area</t>
   </si>
@@ -151,7 +126,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -175,6 +150,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -192,10 +173,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="for_spreadsheet" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -463,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView showRuler="0" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S5" sqref="L5:S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,48 +453,48 @@
     <col min="5" max="5" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -551,7 +528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -1829,12 +1806,12 @@
         <v>1.0119841136212822</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1872,7 +1849,7 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -2459,708 +2436,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>1.8536600000000001</v>
-      </c>
-      <c r="C2">
-        <v>1.36134</v>
-      </c>
-      <c r="D2">
-        <v>1.76471</v>
-      </c>
-      <c r="E2">
-        <v>1.47929</v>
-      </c>
-      <c r="F2">
-        <v>1.74194</v>
-      </c>
-      <c r="G2">
-        <v>1.59535</v>
-      </c>
-      <c r="H2">
-        <v>1.792</v>
-      </c>
-      <c r="I2">
-        <v>1.8202199999999999</v>
-      </c>
-      <c r="J2">
-        <v>1.9230799999999999</v>
-      </c>
-      <c r="K2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1.8</v>
-      </c>
-      <c r="B3">
-        <v>1.14513</v>
-      </c>
-      <c r="C3">
-        <v>1.32582</v>
-      </c>
-      <c r="D3">
-        <v>1.65079</v>
-      </c>
-      <c r="E3">
-        <v>2.0833300000000001</v>
-      </c>
-      <c r="F3">
-        <v>2.5814900000000001</v>
-      </c>
-      <c r="G3">
-        <v>2.4088699999999998</v>
-      </c>
-      <c r="H3">
-        <v>2.68729</v>
-      </c>
-      <c r="I3">
-        <v>3.8282099999999999</v>
-      </c>
-      <c r="J3">
-        <v>3.9929000000000001</v>
-      </c>
-      <c r="K3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1.6</v>
-      </c>
-      <c r="B4">
-        <v>1.1231899999999999</v>
-      </c>
-      <c r="C4">
-        <v>1.34416</v>
-      </c>
-      <c r="D4">
-        <v>1.65079</v>
-      </c>
-      <c r="E4">
-        <v>2.3480699999999999</v>
-      </c>
-      <c r="F4">
-        <v>2.67008</v>
-      </c>
-      <c r="G4">
-        <v>2.47139</v>
-      </c>
-      <c r="H4">
-        <v>2.9592000000000001</v>
-      </c>
-      <c r="I4">
-        <v>2.5920000000000001</v>
-      </c>
-      <c r="J4">
-        <v>2.9729700000000001</v>
-      </c>
-      <c r="K4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1.4</v>
-      </c>
-      <c r="B5">
-        <v>1.1216200000000001</v>
-      </c>
-      <c r="C5">
-        <v>1.36758</v>
-      </c>
-      <c r="D5">
-        <v>1.7885200000000001</v>
-      </c>
-      <c r="E5">
-        <v>1.8594999999999999</v>
-      </c>
-      <c r="F5">
-        <v>1.82741</v>
-      </c>
-      <c r="G5">
-        <v>2.7080299999999999</v>
-      </c>
-      <c r="H5">
-        <v>2.8167900000000001</v>
-      </c>
-      <c r="I5">
-        <v>2.57803</v>
-      </c>
-      <c r="J5">
-        <v>3.74288</v>
-      </c>
-      <c r="K5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1.2</v>
-      </c>
-      <c r="B6">
-        <v>1.1527400000000001</v>
-      </c>
-      <c r="C6">
-        <v>1.5044</v>
-      </c>
-      <c r="D6">
-        <v>1.53975</v>
-      </c>
-      <c r="E6">
-        <v>1.5625</v>
-      </c>
-      <c r="F6">
-        <v>1.7059500000000001</v>
-      </c>
-      <c r="G6">
-        <v>2.13496</v>
-      </c>
-      <c r="H6">
-        <v>2.8054800000000002</v>
-      </c>
-      <c r="I6">
-        <v>2.7930999999999999</v>
-      </c>
-      <c r="J6">
-        <v>2.8664999999999998</v>
-      </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>1.1451199999999999</v>
-      </c>
-      <c r="C7">
-        <v>1.4464300000000001</v>
-      </c>
-      <c r="D7">
-        <v>1.73285</v>
-      </c>
-      <c r="E7">
-        <v>1.7373400000000001</v>
-      </c>
-      <c r="F7">
-        <v>1.73767</v>
-      </c>
-      <c r="G7">
-        <v>2.3857699999999999</v>
-      </c>
-      <c r="H7">
-        <v>2.4763500000000001</v>
-      </c>
-      <c r="I7">
-        <v>2.8114400000000002</v>
-      </c>
-      <c r="J7">
-        <v>3.0713599999999999</v>
-      </c>
-      <c r="K7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>0.8</v>
-      </c>
-      <c r="B8">
-        <v>1.13913</v>
-      </c>
-      <c r="C8">
-        <v>1.4017200000000001</v>
-      </c>
-      <c r="D8">
-        <v>1.4662599999999999</v>
-      </c>
-      <c r="E8">
-        <v>1.4446600000000001</v>
-      </c>
-      <c r="F8">
-        <v>1.5845100000000001</v>
-      </c>
-      <c r="G8">
-        <v>2.2559900000000002</v>
-      </c>
-      <c r="H8">
-        <v>2.3832900000000001</v>
-      </c>
-      <c r="I8">
-        <v>2.5979999999999999</v>
-      </c>
-      <c r="J8">
-        <v>3.3932099999999998</v>
-      </c>
-      <c r="K8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>0.6</v>
-      </c>
-      <c r="B9">
-        <v>1.0531600000000001</v>
-      </c>
-      <c r="C9">
-        <v>1.3052299999999999</v>
-      </c>
-      <c r="D9">
-        <v>1.49264</v>
-      </c>
-      <c r="E9">
-        <v>1.8511</v>
-      </c>
-      <c r="F9">
-        <v>1.5726800000000001</v>
-      </c>
-      <c r="G9">
-        <v>1.81481</v>
-      </c>
-      <c r="H9">
-        <v>1.8073900000000001</v>
-      </c>
-      <c r="I9">
-        <v>2.4187500000000002</v>
-      </c>
-      <c r="J9">
-        <v>2.3648600000000002</v>
-      </c>
-      <c r="K9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0.4</v>
-      </c>
-      <c r="B10">
-        <v>1.09456</v>
-      </c>
-      <c r="C10">
-        <v>1.1939900000000001</v>
-      </c>
-      <c r="D10">
-        <v>1.36528</v>
-      </c>
-      <c r="E10">
-        <v>1.7741</v>
-      </c>
-      <c r="F10">
-        <v>1.7123699999999999</v>
-      </c>
-      <c r="G10">
-        <v>1.8666700000000001</v>
-      </c>
-      <c r="H10">
-        <v>1.5737699999999999</v>
-      </c>
-      <c r="I10">
-        <v>1.7179199999999999</v>
-      </c>
-      <c r="J10">
-        <v>2.2575699999999999</v>
-      </c>
-      <c r="K10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0.2</v>
-      </c>
-      <c r="B11">
-        <v>1.0562100000000001</v>
-      </c>
-      <c r="C11">
-        <v>1.1480999999999999</v>
-      </c>
-      <c r="D11">
-        <v>1.18482</v>
-      </c>
-      <c r="E11">
-        <v>1.3494999999999999</v>
-      </c>
-      <c r="F11">
-        <v>1.62737</v>
-      </c>
-      <c r="G11">
-        <v>1.67045</v>
-      </c>
-      <c r="H11">
-        <v>1.73326</v>
-      </c>
-      <c r="I11">
-        <v>1.5178499999999999</v>
-      </c>
-      <c r="J11">
-        <v>1.71723</v>
-      </c>
-      <c r="K11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>0.1</v>
-      </c>
-      <c r="B12">
-        <v>1.02349</v>
-      </c>
-      <c r="C12">
-        <v>1.0375399999999999</v>
-      </c>
-      <c r="D12">
-        <v>1.1470199999999999</v>
-      </c>
-      <c r="E12">
-        <v>1.2188300000000001</v>
-      </c>
-      <c r="F12">
-        <v>1.2861199999999999</v>
-      </c>
-      <c r="G12">
-        <v>1.33558</v>
-      </c>
-      <c r="H12">
-        <v>1.2548999999999999</v>
-      </c>
-      <c r="I12">
-        <v>1.25709</v>
-      </c>
-      <c r="J12">
-        <v>1.3713900000000001</v>
-      </c>
-      <c r="K12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>0.08</v>
-      </c>
-      <c r="B13">
-        <v>1.0143200000000001</v>
-      </c>
-      <c r="C13">
-        <v>1.0368200000000001</v>
-      </c>
-      <c r="D13">
-        <v>1.0849800000000001</v>
-      </c>
-      <c r="E13">
-        <v>1.1451100000000001</v>
-      </c>
-      <c r="F13">
-        <v>1.20323</v>
-      </c>
-      <c r="G13">
-        <v>1.29548</v>
-      </c>
-      <c r="H13">
-        <v>1.2228300000000001</v>
-      </c>
-      <c r="I13">
-        <v>1.20896</v>
-      </c>
-      <c r="J13">
-        <v>1.25722</v>
-      </c>
-      <c r="K13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>0.06</v>
-      </c>
-      <c r="B14">
-        <v>1.00759</v>
-      </c>
-      <c r="C14">
-        <v>1.03349</v>
-      </c>
-      <c r="D14">
-        <v>1.0370699999999999</v>
-      </c>
-      <c r="E14">
-        <v>1.10328</v>
-      </c>
-      <c r="F14">
-        <v>1.0844400000000001</v>
-      </c>
-      <c r="G14">
-        <v>1.2034800000000001</v>
-      </c>
-      <c r="H14">
-        <v>1.17547</v>
-      </c>
-      <c r="I14">
-        <v>1.26431</v>
-      </c>
-      <c r="J14">
-        <v>1.1868300000000001</v>
-      </c>
-      <c r="K14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>0.05</v>
-      </c>
-      <c r="B15">
-        <v>1.0159199999999999</v>
-      </c>
-      <c r="C15">
-        <v>1.02633</v>
-      </c>
-      <c r="D15">
-        <v>1.0484500000000001</v>
-      </c>
-      <c r="E15">
-        <v>1.0731200000000001</v>
-      </c>
-      <c r="F15">
-        <v>1.0606899999999999</v>
-      </c>
-      <c r="G15">
-        <v>1.12141</v>
-      </c>
-      <c r="H15">
-        <v>1.14801</v>
-      </c>
-      <c r="I15">
-        <v>1.2327399999999999</v>
-      </c>
-      <c r="J15">
-        <v>1.15544</v>
-      </c>
-      <c r="K15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>0.04</v>
-      </c>
-      <c r="B16">
-        <v>1.0027699999999999</v>
-      </c>
-      <c r="C16">
-        <v>1.02755</v>
-      </c>
-      <c r="D16">
-        <v>1.00502</v>
-      </c>
-      <c r="E16">
-        <v>1.05935</v>
-      </c>
-      <c r="F16">
-        <v>1.0763400000000001</v>
-      </c>
-      <c r="G16">
-        <v>1.0701000000000001</v>
-      </c>
-      <c r="H16">
-        <v>1.1327799999999999</v>
-      </c>
-      <c r="I16">
-        <v>1.18068</v>
-      </c>
-      <c r="J16">
-        <v>1.1091299999999999</v>
-      </c>
-      <c r="K16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>0.03</v>
-      </c>
-      <c r="B17">
-        <v>1.0050600000000001</v>
-      </c>
-      <c r="C17">
-        <v>1.0156099999999999</v>
-      </c>
-      <c r="D17">
-        <v>1.01387</v>
-      </c>
-      <c r="E17">
-        <v>1.04257</v>
-      </c>
-      <c r="F17">
-        <v>1.06674</v>
-      </c>
-      <c r="G17">
-        <v>1.0508299999999999</v>
-      </c>
-      <c r="H17">
-        <v>1.3234300000000001</v>
-      </c>
-      <c r="I17">
-        <v>1.1149500000000001</v>
-      </c>
-      <c r="J17">
-        <v>1.0848199999999999</v>
-      </c>
-      <c r="K17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>0.02</v>
-      </c>
-      <c r="B18">
-        <v>1.00587</v>
-      </c>
-      <c r="C18">
-        <v>1.0197400000000001</v>
-      </c>
-      <c r="D18">
-        <v>1.0099800000000001</v>
-      </c>
-      <c r="E18">
-        <v>1.0406899999999999</v>
-      </c>
-      <c r="F18">
-        <v>1.0400100000000001</v>
-      </c>
-      <c r="G18">
-        <v>1.0263800000000001</v>
-      </c>
-      <c r="H18">
-        <v>1.1544700000000001</v>
-      </c>
-      <c r="I18">
-        <v>1.09222</v>
-      </c>
-      <c r="J18">
-        <v>1.0683499999999999</v>
-      </c>
-      <c r="K18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>0.01</v>
-      </c>
-      <c r="B19">
-        <v>1.0023500000000001</v>
-      </c>
-      <c r="C19">
-        <v>1.00874</v>
-      </c>
-      <c r="D19">
-        <v>1.01675</v>
-      </c>
-      <c r="E19">
-        <v>1.01885</v>
-      </c>
-      <c r="F19">
-        <v>1.0234300000000001</v>
-      </c>
-      <c r="G19">
-        <v>1.01902</v>
-      </c>
-      <c r="H19">
-        <v>1.28898</v>
-      </c>
-      <c r="I19">
-        <v>1.0397400000000001</v>
-      </c>
-      <c r="J19">
-        <v>1.0155700000000001</v>
-      </c>
-      <c r="K19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:U20"/>
+    <sheetView showRuler="0" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -5117,4 +4412,1233 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2.2387999999999999</v>
+      </c>
+      <c r="C2" s="10">
+        <v>2.2448700000000001</v>
+      </c>
+      <c r="D2" s="10">
+        <v>2.2819799999999999</v>
+      </c>
+      <c r="E2" s="10">
+        <v>2.2716400000000001</v>
+      </c>
+      <c r="F2" s="10">
+        <v>2.2429199999999998</v>
+      </c>
+      <c r="G2" s="10">
+        <v>2.2909999999999999</v>
+      </c>
+      <c r="H2" s="10">
+        <v>2.3243900000000002</v>
+      </c>
+      <c r="I2" s="10">
+        <v>2.2610899999999998</v>
+      </c>
+      <c r="J2" s="10">
+        <v>2.2938200000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2.1290100000000001</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2.12887</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2.1581700000000001</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2.4160400000000002</v>
+      </c>
+      <c r="F3" s="10">
+        <v>2.1287099999999999</v>
+      </c>
+      <c r="G3" s="10">
+        <v>2.4259599999999999</v>
+      </c>
+      <c r="H3" s="10">
+        <v>2.2274799999999999</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2.17028</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2.6488700000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2.1125699999999998</v>
+      </c>
+      <c r="C4" s="10">
+        <v>2.1158999999999999</v>
+      </c>
+      <c r="D4" s="10">
+        <v>2.14696</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2.39974</v>
+      </c>
+      <c r="F4" s="10">
+        <v>2.1149</v>
+      </c>
+      <c r="G4" s="10">
+        <v>2.4179400000000002</v>
+      </c>
+      <c r="H4" s="10">
+        <v>2.22119</v>
+      </c>
+      <c r="I4" s="10">
+        <v>2.1590500000000001</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2.6342500000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2.0924900000000002</v>
+      </c>
+      <c r="C5" s="10">
+        <v>2.0950899999999999</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2.1273499999999999</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2.37995</v>
+      </c>
+      <c r="F5" s="10">
+        <v>2.0965400000000001</v>
+      </c>
+      <c r="G5" s="10">
+        <v>2.3945799999999999</v>
+      </c>
+      <c r="H5" s="10">
+        <v>2.1991800000000001</v>
+      </c>
+      <c r="I5" s="10">
+        <v>2.1194500000000001</v>
+      </c>
+      <c r="J5" s="10">
+        <v>2.60765</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>1.2</v>
+      </c>
+      <c r="B6" s="10">
+        <v>2.06941</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2.07396</v>
+      </c>
+      <c r="D6" s="10">
+        <v>2.1059100000000002</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2.3524099999999999</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2.0788899999999999</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2.3683700000000001</v>
+      </c>
+      <c r="H6" s="10">
+        <v>2.18222</v>
+      </c>
+      <c r="I6" s="10">
+        <v>2.1055999999999999</v>
+      </c>
+      <c r="J6" s="10">
+        <v>2.5886200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10">
+        <v>2.0359400000000001</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2.0385399999999998</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2.0686</v>
+      </c>
+      <c r="E7" s="10">
+        <v>2.31758</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2.0392899999999998</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2.3337400000000001</v>
+      </c>
+      <c r="H7" s="10">
+        <v>2.1462699999999999</v>
+      </c>
+      <c r="I7" s="10">
+        <v>2.0800299999999998</v>
+      </c>
+      <c r="J7" s="10">
+        <v>2.5394399999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1.98966</v>
+      </c>
+      <c r="C8" s="10">
+        <v>1.99132</v>
+      </c>
+      <c r="D8" s="10">
+        <v>2.02149</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2.2658</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1.99353</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2.28207</v>
+      </c>
+      <c r="H8" s="10">
+        <v>2.09897</v>
+      </c>
+      <c r="I8" s="10">
+        <v>2.0347300000000001</v>
+      </c>
+      <c r="J8" s="10">
+        <v>2.4980000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1.9115599999999999</v>
+      </c>
+      <c r="C9" s="10">
+        <v>1.92041</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1.94957</v>
+      </c>
+      <c r="E9" s="10">
+        <v>2.18397</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1.92049</v>
+      </c>
+      <c r="G9" s="10">
+        <v>2.2048899999999998</v>
+      </c>
+      <c r="H9" s="10">
+        <v>2.0303300000000002</v>
+      </c>
+      <c r="I9" s="10">
+        <v>1.9577199999999999</v>
+      </c>
+      <c r="J9" s="10">
+        <v>2.4080599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1.7803199999999999</v>
+      </c>
+      <c r="C10" s="10">
+        <v>1.7874000000000001</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1.8157300000000001</v>
+      </c>
+      <c r="E10" s="10">
+        <v>2.0424500000000001</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1.79217</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2.0579499999999999</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1.9017999999999999</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1.8301700000000001</v>
+      </c>
+      <c r="J10" s="10">
+        <v>2.266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1.4696100000000001</v>
+      </c>
+      <c r="C11" s="10">
+        <v>1.4782</v>
+      </c>
+      <c r="D11" s="10">
+        <v>1.5054399999999999</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.7019</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1.48621</v>
+      </c>
+      <c r="G11" s="10">
+        <v>1.7233799999999999</v>
+      </c>
+      <c r="H11" s="10">
+        <v>1.59005</v>
+      </c>
+      <c r="I11" s="10">
+        <v>1.52214</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1.9089</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1.08876</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1.1045199999999999</v>
+      </c>
+      <c r="D12" s="10">
+        <v>1.11934</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1.2786900000000001</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1.1092900000000001</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1.29461</v>
+      </c>
+      <c r="H12" s="10">
+        <v>1.2074499999999999</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1.15883</v>
+      </c>
+      <c r="J12" s="10">
+        <v>1.4454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="B13" s="10">
+        <v>1.02525</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1.0178799999999999</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1.03281</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.1333500000000001</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1.0204800000000001</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1.1549</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1.0693699999999999</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1.0283</v>
+      </c>
+      <c r="J13" s="10">
+        <v>1.3106500000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="B14" s="10">
+        <v>1.0265200000000001</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1.0351300000000001</v>
+      </c>
+      <c r="D14" s="10">
+        <v>1.03912</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1.1480300000000001</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1.04301</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1.1844300000000001</v>
+      </c>
+      <c r="H14" s="10">
+        <v>1.0914200000000001</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1.0811299999999999</v>
+      </c>
+      <c r="J14" s="10">
+        <v>1.2811999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="B15" s="10">
+        <v>1.02156</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1.0203599999999999</v>
+      </c>
+      <c r="D15" s="10">
+        <v>1.0339400000000001</v>
+      </c>
+      <c r="E15" s="10">
+        <v>1.10585</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1.0323599999999999</v>
+      </c>
+      <c r="G15" s="10">
+        <v>1.12652</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1.0852999999999999</v>
+      </c>
+      <c r="I15" s="10">
+        <v>1.06132</v>
+      </c>
+      <c r="J15" s="10">
+        <v>1.20445</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>0.04</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1.0587800000000001</v>
+      </c>
+      <c r="C16" s="10">
+        <v>1.06027</v>
+      </c>
+      <c r="D16" s="10">
+        <v>1.06138</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1.12093</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1.07599</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1.1172500000000001</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1.09212</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1.1008899999999999</v>
+      </c>
+      <c r="J16" s="10">
+        <v>1.19885</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1.0768599999999999</v>
+      </c>
+      <c r="C17" s="10">
+        <v>1.0784899999999999</v>
+      </c>
+      <c r="D17" s="10">
+        <v>1.09049</v>
+      </c>
+      <c r="E17" s="10">
+        <v>1.1176900000000001</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1.0956699999999999</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1.10833</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="10">
+        <v>1.1139600000000001</v>
+      </c>
+      <c r="J17" s="10">
+        <v>1.15323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="B18" s="10">
+        <v>1.02372</v>
+      </c>
+      <c r="C18" s="10">
+        <v>1.0344599999999999</v>
+      </c>
+      <c r="D18" s="10">
+        <v>1.03125</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1.0266299999999999</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1.0289699999999999</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1.0297000000000001</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J18" s="10">
+        <v>1.0556099999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10">
+        <v>1.0296799999999999</v>
+      </c>
+      <c r="D19" s="10">
+        <v>1.03037</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1.0415399999999999</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1.03033</v>
+      </c>
+      <c r="G19" s="10">
+        <v>1.0445199999999999</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="10">
+        <v>1.04718</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.0021</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.00915</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.04026</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.04545</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.00726</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1.06416</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1.0555600000000001</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1.05646</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1.08009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1.01736</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.02512</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.14608</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.2096199999999999</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.19994</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1.2312799999999999</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1.36463</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1.4151</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1.53711</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>1.6</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1.0276400000000001</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.0416000000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1.07823</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.1974100000000001</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1.1811199999999999</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1.23132</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.5362499999999999</v>
+      </c>
+      <c r="I24" s="2">
+        <v>1.6864600000000001</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1.5772299999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.0180800000000001</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.05602</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.0904799999999999</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1.2463</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1.31535</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1.3862000000000001</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1.36694</v>
+      </c>
+      <c r="I25" s="2">
+        <v>1.5220400000000001</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1.6192299999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1.0254300000000001</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1.06426</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.2415</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.2375</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1.29511</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1.32423</v>
+      </c>
+      <c r="H26" s="2">
+        <v>1.4754799999999999</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1.5619099999999999</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1.8443099999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1.0214399999999999</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.0491200000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.15272</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1.2534000000000001</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1.3088</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1.34945</v>
+      </c>
+      <c r="H27" s="2">
+        <v>1.4889300000000001</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.7964500000000001</v>
+      </c>
+      <c r="J27" s="2">
+        <v>2.1539199999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.04183</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.0573600000000001</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.0995299999999999</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.22584</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.2693099999999999</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1.5272399999999999</v>
+      </c>
+      <c r="H28" s="2">
+        <v>1.7924100000000001</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1.8368800000000001</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.9527699999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.03434</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.1119000000000001</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.13361</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1.3811100000000001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1.5101199999999999</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1.6071800000000001</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1.7881100000000001</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1.9577199999999999</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2.1670400000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.0419799999999999</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1.18544</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.2623800000000001</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1.38568</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1.65984</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1.4663200000000001</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1.9017999999999999</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1.8301700000000001</v>
+      </c>
+      <c r="J30" s="2">
+        <v>2.266</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1.05681</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1.16601</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1.16073</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1.32942</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1.48621</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1.62486</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.59005</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1.52214</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1.7780400000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1.08876</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.1045199999999999</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.11934</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1.13618</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1.1092900000000001</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1.19184</v>
+      </c>
+      <c r="H32" s="2">
+        <v>1.2074499999999999</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1.15883</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1.19371</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.02525</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1.0178799999999999</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1.03281</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1.1333500000000001</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1.0204800000000001</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1.1549</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.0693699999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1.0283</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1.1406700000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.0265200000000001</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.0351300000000001</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.03912</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1.1480300000000001</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1.04301</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1.1844300000000001</v>
+      </c>
+      <c r="H34" s="2">
+        <v>1.0914200000000001</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1.0811299999999999</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1.2811999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1.02156</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1.0203599999999999</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1.0339400000000001</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1.10585</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1.0323599999999999</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1.12652</v>
+      </c>
+      <c r="H35" s="2">
+        <v>1.0852999999999999</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.06132</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.20445</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1.0587800000000001</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1.06027</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1.06138</v>
+      </c>
+      <c r="E36" s="2">
+        <v>1.12093</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1.07599</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1.1172500000000001</v>
+      </c>
+      <c r="H36" s="2">
+        <v>1.09212</v>
+      </c>
+      <c r="I36" s="2">
+        <v>1.1008899999999999</v>
+      </c>
+      <c r="J36" s="2">
+        <v>1.19885</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1.0768599999999999</v>
+      </c>
+      <c r="C37" s="2">
+        <v>1.0784899999999999</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1.09049</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1.1176900000000001</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1.0956699999999999</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1.10833</v>
+      </c>
+      <c r="H37" s="2">
+        <v>1.09948</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1.1139600000000001</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1.15323</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.02372</v>
+      </c>
+      <c r="C38" s="2">
+        <v>1.0344599999999999</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1.03125</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1.0266299999999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>1.0289699999999999</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1.0297000000000001</v>
+      </c>
+      <c r="H38" s="2">
+        <v>1.0292300000000001</v>
+      </c>
+      <c r="I38" s="2">
+        <v>1.0338400000000001</v>
+      </c>
+      <c r="J38" s="2">
+        <v>1.0556099999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1.0302800000000001</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1.0296799999999999</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1.03037</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1.0415399999999999</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1.03033</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.0445199999999999</v>
+      </c>
+      <c r="H39" s="2">
+        <v>1.0378799999999999</v>
+      </c>
+      <c r="I39" s="2">
+        <v>1.03477</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1.04718</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added appendices and finished results.
</commit_message>
<xml_diff>
--- a/MetricConvergence.xlsx
+++ b/MetricConvergence.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="14320" windowWidth="24720" windowHeight="13340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="16160" yWindow="460" windowWidth="34220" windowHeight="20280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Opposite Pins" sheetId="1" r:id="rId1"/>
-    <sheet name="Same Side Pins" sheetId="2" r:id="rId2"/>
-    <sheet name="Lattice" sheetId="5" r:id="rId3"/>
+    <sheet name="opp_no_iter" sheetId="6" r:id="rId2"/>
+    <sheet name="Same Side Pins" sheetId="2" r:id="rId3"/>
+    <sheet name="Lattice" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="12">
   <si>
     <t>Area</t>
   </si>
@@ -123,7 +124,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -149,6 +150,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S5" sqref="L5:S5"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,17 +455,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2230,7 +2234,7 @@
         <v>1.3814500000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>0.06</v>
       </c>
@@ -2262,7 +2266,7 @@
         <v>1.0684100000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>0.05</v>
       </c>
@@ -2433,6 +2437,629 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection sqref="A1:J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1.9487000000000001</v>
+      </c>
+      <c r="C2">
+        <v>4.1204000000000001</v>
+      </c>
+      <c r="D2">
+        <v>6.7554999999999996</v>
+      </c>
+      <c r="E2">
+        <v>9.5959000000000003</v>
+      </c>
+      <c r="F2">
+        <v>12.436</v>
+      </c>
+      <c r="G2">
+        <v>14.212999999999999</v>
+      </c>
+      <c r="H2">
+        <v>16.443999999999999</v>
+      </c>
+      <c r="I2">
+        <v>8.5976999999999997</v>
+      </c>
+      <c r="J2" s="2">
+        <v>6.7708300000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="B3">
+        <v>1.4575</v>
+      </c>
+      <c r="C3">
+        <v>2.3248000000000002</v>
+      </c>
+      <c r="D3">
+        <v>4.1120999999999999</v>
+      </c>
+      <c r="E3">
+        <v>4.6428000000000003</v>
+      </c>
+      <c r="F3">
+        <v>7.8387000000000002</v>
+      </c>
+      <c r="G3">
+        <v>8.6068999999999996</v>
+      </c>
+      <c r="H3">
+        <v>24.765000000000001</v>
+      </c>
+      <c r="I3">
+        <v>6.1363000000000003</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4.5774600000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="B4">
+        <v>1.4227000000000001</v>
+      </c>
+      <c r="C4">
+        <v>2.2132999999999998</v>
+      </c>
+      <c r="D4">
+        <v>4.2027000000000001</v>
+      </c>
+      <c r="E4">
+        <v>4.6428000000000003</v>
+      </c>
+      <c r="F4">
+        <v>6.8571</v>
+      </c>
+      <c r="G4">
+        <v>8.5180000000000007</v>
+      </c>
+      <c r="H4">
+        <v>24.715</v>
+      </c>
+      <c r="I4">
+        <v>5.9383999999999997</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4.5774600000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>1.4</v>
+      </c>
+      <c r="B5">
+        <v>1.3162</v>
+      </c>
+      <c r="C5">
+        <v>2.0535999999999999</v>
+      </c>
+      <c r="D5">
+        <v>2.9779</v>
+      </c>
+      <c r="E5">
+        <v>4.6428000000000003</v>
+      </c>
+      <c r="F5">
+        <v>6.2306999999999997</v>
+      </c>
+      <c r="G5">
+        <v>8.5770999999999997</v>
+      </c>
+      <c r="H5">
+        <v>19.983000000000001</v>
+      </c>
+      <c r="I5">
+        <v>5.9036999999999997</v>
+      </c>
+      <c r="J5" s="2">
+        <v>4.51389</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>1.2</v>
+      </c>
+      <c r="B6">
+        <v>1.2976000000000001</v>
+      </c>
+      <c r="C6">
+        <v>1.9523999999999999</v>
+      </c>
+      <c r="D6">
+        <v>3.0215999999999998</v>
+      </c>
+      <c r="E6">
+        <v>4.9295</v>
+      </c>
+      <c r="F6">
+        <v>4.5050999999999997</v>
+      </c>
+      <c r="G6">
+        <v>7.2458999999999998</v>
+      </c>
+      <c r="H6">
+        <v>19.972999999999999</v>
+      </c>
+      <c r="I6">
+        <v>4.2992999999999997</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4.51389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1.3476999999999999</v>
+      </c>
+      <c r="C7">
+        <v>1.7544</v>
+      </c>
+      <c r="D7">
+        <v>2.9028999999999998</v>
+      </c>
+      <c r="E7">
+        <v>4.9295</v>
+      </c>
+      <c r="F7">
+        <v>4.5205000000000002</v>
+      </c>
+      <c r="G7">
+        <v>6.0225999999999997</v>
+      </c>
+      <c r="H7">
+        <v>20.013000000000002</v>
+      </c>
+      <c r="I7">
+        <v>4.6188000000000002</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4.51389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="B8">
+        <v>1.2566999999999999</v>
+      </c>
+      <c r="C8">
+        <v>1.6526000000000001</v>
+      </c>
+      <c r="D8">
+        <v>2.9497</v>
+      </c>
+      <c r="E8">
+        <v>3.3111999999999999</v>
+      </c>
+      <c r="F8">
+        <v>4.4511000000000003</v>
+      </c>
+      <c r="G8">
+        <v>4.4001000000000001</v>
+      </c>
+      <c r="H8">
+        <v>19.739000000000001</v>
+      </c>
+      <c r="I8">
+        <v>4.5849000000000002</v>
+      </c>
+      <c r="J8" s="2">
+        <v>2.9166699999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="B9">
+        <v>1.1423000000000001</v>
+      </c>
+      <c r="C9">
+        <v>1.4516</v>
+      </c>
+      <c r="D9">
+        <v>2.0545</v>
+      </c>
+      <c r="E9">
+        <v>3.0059999999999998</v>
+      </c>
+      <c r="F9">
+        <v>3.5497000000000001</v>
+      </c>
+      <c r="G9">
+        <v>4.2241</v>
+      </c>
+      <c r="H9">
+        <v>14.28</v>
+      </c>
+      <c r="I9">
+        <v>2.8738000000000001</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3.09917</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B10">
+        <v>1.0945</v>
+      </c>
+      <c r="C10">
+        <v>1.3529</v>
+      </c>
+      <c r="D10">
+        <v>1.7867999999999999</v>
+      </c>
+      <c r="E10">
+        <v>2.0213999999999999</v>
+      </c>
+      <c r="F10">
+        <v>2.7378999999999998</v>
+      </c>
+      <c r="G10">
+        <v>3.3302999999999998</v>
+      </c>
+      <c r="H10">
+        <v>14.093</v>
+      </c>
+      <c r="I10">
+        <v>2.8027000000000002</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2.06311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B11">
+        <v>1.0457000000000001</v>
+      </c>
+      <c r="C11">
+        <v>1.1361000000000001</v>
+      </c>
+      <c r="D11">
+        <v>1.3358000000000001</v>
+      </c>
+      <c r="E11">
+        <v>1.5451999999999999</v>
+      </c>
+      <c r="F11">
+        <v>1.6476</v>
+      </c>
+      <c r="G11">
+        <v>2.0493999999999999</v>
+      </c>
+      <c r="H11">
+        <v>8.7796000000000003</v>
+      </c>
+      <c r="I11">
+        <v>1.8173999999999999</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.4455800000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B12">
+        <v>1.0197000000000001</v>
+      </c>
+      <c r="C12">
+        <v>1.0426</v>
+      </c>
+      <c r="D12">
+        <v>1.1093</v>
+      </c>
+      <c r="E12">
+        <v>1.1698</v>
+      </c>
+      <c r="F12">
+        <v>1.2868999999999999</v>
+      </c>
+      <c r="G12">
+        <v>1.3647</v>
+      </c>
+      <c r="H12">
+        <v>4.4272999999999998</v>
+      </c>
+      <c r="I12">
+        <v>1.4091</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1.2449399999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>0.08</v>
+      </c>
+      <c r="B13">
+        <v>1.0112000000000001</v>
+      </c>
+      <c r="C13">
+        <v>1.0290999999999999</v>
+      </c>
+      <c r="D13">
+        <v>1.0943000000000001</v>
+      </c>
+      <c r="E13">
+        <v>1.19</v>
+      </c>
+      <c r="F13">
+        <v>1.2085999999999999</v>
+      </c>
+      <c r="G13">
+        <v>1.2899</v>
+      </c>
+      <c r="H13">
+        <v>3.3851</v>
+      </c>
+      <c r="I13">
+        <v>1.3178000000000001</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1.1760200000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="B14">
+        <v>1.0052000000000001</v>
+      </c>
+      <c r="C14">
+        <v>1.0305</v>
+      </c>
+      <c r="D14">
+        <v>1.0373000000000001</v>
+      </c>
+      <c r="E14">
+        <v>1.1048</v>
+      </c>
+      <c r="F14">
+        <v>1.0866</v>
+      </c>
+      <c r="G14">
+        <v>1.1980999999999999</v>
+      </c>
+      <c r="H14">
+        <v>2.9331</v>
+      </c>
+      <c r="I14">
+        <v>1.2828999999999999</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1.0634699999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="B15">
+        <v>1.0206</v>
+      </c>
+      <c r="C15">
+        <v>1.0216000000000001</v>
+      </c>
+      <c r="D15">
+        <v>1.0575000000000001</v>
+      </c>
+      <c r="E15">
+        <v>1.0915999999999999</v>
+      </c>
+      <c r="F15">
+        <v>1.0791999999999999</v>
+      </c>
+      <c r="G15">
+        <v>1.1146</v>
+      </c>
+      <c r="H15">
+        <v>2.6072000000000002</v>
+      </c>
+      <c r="I15">
+        <v>1.2175</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1.0866199999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="B16">
+        <v>1.004</v>
+      </c>
+      <c r="C16">
+        <v>1.0134000000000001</v>
+      </c>
+      <c r="D16">
+        <v>1.0016</v>
+      </c>
+      <c r="E16">
+        <v>1.0608</v>
+      </c>
+      <c r="F16">
+        <v>1.0734999999999999</v>
+      </c>
+      <c r="G16">
+        <v>1.0730999999999999</v>
+      </c>
+      <c r="H16">
+        <v>2.2021999999999999</v>
+      </c>
+      <c r="I16">
+        <v>1.1711</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.1099600000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="B17">
+        <v>1.0028999999999999</v>
+      </c>
+      <c r="C17">
+        <v>1.0164</v>
+      </c>
+      <c r="D17">
+        <v>1.0207999999999999</v>
+      </c>
+      <c r="E17">
+        <v>1.0499000000000001</v>
+      </c>
+      <c r="F17">
+        <v>1.0650999999999999</v>
+      </c>
+      <c r="G17">
+        <v>1.0479000000000001</v>
+      </c>
+      <c r="H17">
+        <v>1.9293</v>
+      </c>
+      <c r="I17">
+        <v>1.1315</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1.03406</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="B18">
+        <v>1.0041</v>
+      </c>
+      <c r="C18">
+        <v>1.0082</v>
+      </c>
+      <c r="D18">
+        <v>1.0099</v>
+      </c>
+      <c r="E18">
+        <v>1.0337000000000001</v>
+      </c>
+      <c r="F18">
+        <v>1.024</v>
+      </c>
+      <c r="G18">
+        <v>1.0275000000000001</v>
+      </c>
+      <c r="H18">
+        <v>1.5743</v>
+      </c>
+      <c r="I18">
+        <v>1.0798000000000001</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.0485500000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="B19">
+        <v>1.0025999999999999</v>
+      </c>
+      <c r="C19">
+        <v>1.0101</v>
+      </c>
+      <c r="D19">
+        <v>1.0082</v>
+      </c>
+      <c r="E19">
+        <v>1.0087999999999999</v>
+      </c>
+      <c r="F19">
+        <v>1.0390999999999999</v>
+      </c>
+      <c r="G19">
+        <v>1.018</v>
+      </c>
+      <c r="H19">
+        <v>1.2765</v>
+      </c>
+      <c r="I19">
+        <v>1.0428999999999999</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.0096700000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U40"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
@@ -2442,17 +3069,17 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -4411,12 +5038,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection sqref="A1:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>